<commit_message>
Added CAN messages for the BMS
Added CAN messages for the BMS
</commit_message>
<xml_diff>
--- a/ION CAN Messages.xlsx
+++ b/ION CAN Messages.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Export Summary" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="176">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -387,13 +387,178 @@
   </si>
   <si>
     <t>Calculated power usage</t>
+  </si>
+  <si>
+    <t>BMS</t>
+  </si>
+  <si>
+    <t>Timer[16:8]</t>
+  </si>
+  <si>
+    <t>Timer[8:0]</t>
+  </si>
+  <si>
+    <t>State[8:0]</t>
+  </si>
+  <si>
+    <t>Flags[8:0]</t>
+  </si>
+  <si>
+    <t>DTC[8:0]</t>
+  </si>
+  <si>
+    <t>Voltage[16:8]</t>
+  </si>
+  <si>
+    <t>Voltage[8:0]</t>
+  </si>
+  <si>
+    <t>Min Vtg[8:0]</t>
+  </si>
+  <si>
+    <t>Min Vtg#[8:0]</t>
+  </si>
+  <si>
+    <t>Max Vtg[8:0]</t>
+  </si>
+  <si>
+    <t>Max Vtg#[8:0]</t>
+  </si>
+  <si>
+    <t>Current[16:8]</t>
+  </si>
+  <si>
+    <t>Current[8:0]</t>
+  </si>
+  <si>
+    <t>Charge Limit[8:0]</t>
+  </si>
+  <si>
+    <t>Charge Limit[16:8]</t>
+  </si>
+  <si>
+    <t>Discharge Limit[16:8]</t>
+  </si>
+  <si>
+    <t>Discharge Limit[8:0]</t>
+  </si>
+  <si>
+    <t>Batt.energy in[32:24]</t>
+  </si>
+  <si>
+    <t>Batt.energy in[24:16]</t>
+  </si>
+  <si>
+    <t>Batt.energy in[16:8]</t>
+  </si>
+  <si>
+    <t>Batt.energy in[8:0]</t>
+  </si>
+  <si>
+    <t>Batt.energy out[32:24]</t>
+  </si>
+  <si>
+    <t>Batt.energy out[24:16]</t>
+  </si>
+  <si>
+    <t>Batt.energy out[16:8]</t>
+  </si>
+  <si>
+    <t>Batt.energy out[8:0]</t>
+  </si>
+  <si>
+    <t>SOC[8:0]</t>
+  </si>
+  <si>
+    <t>DOD[8:0]</t>
+  </si>
+  <si>
+    <t>Capacity[16:8]</t>
+  </si>
+  <si>
+    <t>Capacity[8:0]</t>
+  </si>
+  <si>
+    <t>SOC2[8:0]</t>
+  </si>
+  <si>
+    <t>SOH[8:0]</t>
+  </si>
+  <si>
+    <t>DOD[16:8]</t>
+  </si>
+  <si>
+    <t>Temperature[8:0]</t>
+  </si>
+  <si>
+    <t>Air temp[8:0]</t>
+  </si>
+  <si>
+    <t>0x620</t>
+  </si>
+  <si>
+    <t>0x621</t>
+  </si>
+  <si>
+    <t>0x622</t>
+  </si>
+  <si>
+    <t>0x623</t>
+  </si>
+  <si>
+    <t>0x624</t>
+  </si>
+  <si>
+    <t>0x625</t>
+  </si>
+  <si>
+    <t>0x626</t>
+  </si>
+  <si>
+    <t>0x627</t>
+  </si>
+  <si>
+    <t>0x628</t>
+  </si>
+  <si>
+    <t>Min tmp[8:0]</t>
+  </si>
+  <si>
+    <t>Min tmp#[8:0]</t>
+  </si>
+  <si>
+    <t>Max tmp[8:0]</t>
+  </si>
+  <si>
+    <t>Max tmp#[8:0]</t>
+  </si>
+  <si>
+    <t>Resistance[16:8]</t>
+  </si>
+  <si>
+    <t>Resistance[8:0]</t>
+  </si>
+  <si>
+    <t>Min res[8:0]</t>
+  </si>
+  <si>
+    <t>Min res#[8:0]</t>
+  </si>
+  <si>
+    <t>Max res[8:0]</t>
+  </si>
+  <si>
+    <t>Max res#[8:0]</t>
+  </si>
+  <si>
+    <t>Descriptions: http://lithiumate.elithion.com/php/controller_can_specs.php</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -431,8 +596,14 @@
       <sz val="10"/>
       <name val="Helvetica"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -511,8 +682,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -535,13 +718,80 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -618,16 +868,61 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -751,7 +1046,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-            <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" val="1"/>
+            <ma14:wrappingTextBoxFlag xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
           </a:ext>
         </a:extLst>
       </xdr:spPr>
@@ -2054,11 +2349,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
     </row>
     <row r="7" spans="2:4" ht="18" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
@@ -2150,13 +2445,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IV42"/>
+  <dimension ref="A1:IZ46"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="E31" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomRight" activeCell="M38" sqref="M38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2166,23 +2461,28 @@
     <col min="3" max="3" width="7.796875" style="6" customWidth="1"/>
     <col min="4" max="4" width="11.796875" style="6" customWidth="1"/>
     <col min="5" max="7" width="10.3984375" style="6" customWidth="1"/>
-    <col min="8" max="8" width="42.796875" style="6" customWidth="1"/>
-    <col min="9" max="256" width="9.09765625" style="6" customWidth="1"/>
+    <col min="8" max="11" width="10.3984375" style="27" customWidth="1"/>
+    <col min="12" max="12" width="42.796875" style="6" customWidth="1"/>
+    <col min="13" max="260" width="9.09765625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:256" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:260" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-    </row>
-    <row r="2" spans="1:256" ht="20.65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+    </row>
+    <row r="2" spans="1:260" ht="20.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>7</v>
       </c>
@@ -2204,11 +2504,23 @@
       <c r="G2" s="7">
         <v>3</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="7">
+        <v>4</v>
+      </c>
+      <c r="I2" s="7">
+        <v>5</v>
+      </c>
+      <c r="J2" s="7">
+        <v>6</v>
+      </c>
+      <c r="K2" s="7">
+        <v>7</v>
+      </c>
+      <c r="L2" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:256" ht="20.65" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:260" ht="20.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>12</v>
       </c>
@@ -2224,12 +2536,16 @@
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:256" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="30" t="s">
+    <row r="4" spans="1:260" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="28" t="s">
         <v>99</v>
       </c>
       <c r="B4" s="9" t="s">
@@ -2240,12 +2556,16 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="9" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:256" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="30" t="s">
+    <row r="5" spans="1:260" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="28" t="s">
         <v>100</v>
       </c>
       <c r="B5" s="10" t="s">
@@ -2256,12 +2576,16 @@
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="9" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="6" spans="1:256" s="1" customFormat="1" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="30" t="s">
+    <row r="6" spans="1:260" s="1" customFormat="1" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="28" t="s">
         <v>101</v>
       </c>
       <c r="B6" s="10" t="s">
@@ -2272,13 +2596,13 @@
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="I6" s="27"/>
-      <c r="J6" s="27"/>
-      <c r="K6" s="27"/>
-      <c r="L6" s="27"/>
       <c r="M6" s="27"/>
       <c r="N6" s="27"/>
       <c r="O6" s="27"/>
@@ -2523,9 +2847,13 @@
       <c r="IT6" s="27"/>
       <c r="IU6" s="27"/>
       <c r="IV6" s="27"/>
-    </row>
-    <row r="7" spans="1:256" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="30" t="s">
+      <c r="IW6" s="27"/>
+      <c r="IX6" s="27"/>
+      <c r="IY6" s="27"/>
+      <c r="IZ6" s="27"/>
+    </row>
+    <row r="7" spans="1:260" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="28" t="s">
         <v>102</v>
       </c>
       <c r="B7" s="10" t="s">
@@ -2536,12 +2864,16 @@
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="9" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="8" spans="1:256" s="1" customFormat="1" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="30" t="s">
+    <row r="8" spans="1:260" s="1" customFormat="1" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="28" t="s">
         <v>103</v>
       </c>
       <c r="B8" s="10" t="s">
@@ -2552,13 +2884,13 @@
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
-      <c r="H8" s="9" t="s">
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="I8" s="27"/>
-      <c r="J8" s="27"/>
-      <c r="K8" s="27"/>
-      <c r="L8" s="27"/>
       <c r="M8" s="27"/>
       <c r="N8" s="27"/>
       <c r="O8" s="27"/>
@@ -2803,9 +3135,13 @@
       <c r="IT8" s="27"/>
       <c r="IU8" s="27"/>
       <c r="IV8" s="27"/>
-    </row>
-    <row r="9" spans="1:256" s="1" customFormat="1" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="31" t="s">
+      <c r="IW8" s="27"/>
+      <c r="IX8" s="27"/>
+      <c r="IY8" s="27"/>
+      <c r="IZ8" s="27"/>
+    </row>
+    <row r="9" spans="1:260" s="1" customFormat="1" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="29" t="s">
         <v>104</v>
       </c>
       <c r="B9" s="10" t="s">
@@ -2816,13 +3152,13 @@
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
-      <c r="H9" s="9" t="s">
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="I9" s="27"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="27"/>
-      <c r="L9" s="27"/>
       <c r="M9" s="27"/>
       <c r="N9" s="27"/>
       <c r="O9" s="27"/>
@@ -3067,9 +3403,13 @@
       <c r="IT9" s="27"/>
       <c r="IU9" s="27"/>
       <c r="IV9" s="27"/>
-    </row>
-    <row r="10" spans="1:256" s="1" customFormat="1" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="30" t="s">
+      <c r="IW9" s="27"/>
+      <c r="IX9" s="27"/>
+      <c r="IY9" s="27"/>
+      <c r="IZ9" s="27"/>
+    </row>
+    <row r="10" spans="1:260" s="1" customFormat="1" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="28" t="s">
         <v>105</v>
       </c>
       <c r="B10" s="10" t="s">
@@ -3080,13 +3420,13 @@
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
-      <c r="H10" s="9" t="s">
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="I10" s="27"/>
-      <c r="J10" s="27"/>
-      <c r="K10" s="27"/>
-      <c r="L10" s="27"/>
       <c r="M10" s="27"/>
       <c r="N10" s="27"/>
       <c r="O10" s="27"/>
@@ -3331,9 +3671,13 @@
       <c r="IT10" s="27"/>
       <c r="IU10" s="27"/>
       <c r="IV10" s="27"/>
-    </row>
-    <row r="11" spans="1:256" s="1" customFormat="1" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="30" t="s">
+      <c r="IW10" s="27"/>
+      <c r="IX10" s="27"/>
+      <c r="IY10" s="27"/>
+      <c r="IZ10" s="27"/>
+    </row>
+    <row r="11" spans="1:260" s="1" customFormat="1" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="28" t="s">
         <v>106</v>
       </c>
       <c r="B11" s="10" t="s">
@@ -3344,13 +3688,13 @@
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
-      <c r="H11" s="9" t="s">
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="I11" s="27"/>
-      <c r="J11" s="27"/>
-      <c r="K11" s="27"/>
-      <c r="L11" s="27"/>
       <c r="M11" s="27"/>
       <c r="N11" s="27"/>
       <c r="O11" s="27"/>
@@ -3595,9 +3939,13 @@
       <c r="IT11" s="27"/>
       <c r="IU11" s="27"/>
       <c r="IV11" s="27"/>
-    </row>
-    <row r="12" spans="1:256" s="1" customFormat="1" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="30" t="s">
+      <c r="IW11" s="27"/>
+      <c r="IX11" s="27"/>
+      <c r="IY11" s="27"/>
+      <c r="IZ11" s="27"/>
+    </row>
+    <row r="12" spans="1:260" s="1" customFormat="1" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="28" t="s">
         <v>107</v>
       </c>
       <c r="B12" s="10" t="s">
@@ -3608,13 +3956,13 @@
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
-      <c r="H12" s="9" t="s">
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="I12" s="27"/>
-      <c r="J12" s="27"/>
-      <c r="K12" s="27"/>
-      <c r="L12" s="27"/>
       <c r="M12" s="27"/>
       <c r="N12" s="27"/>
       <c r="O12" s="27"/>
@@ -3859,9 +4207,13 @@
       <c r="IT12" s="27"/>
       <c r="IU12" s="27"/>
       <c r="IV12" s="27"/>
-    </row>
-    <row r="13" spans="1:256" s="1" customFormat="1" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="30" t="s">
+      <c r="IW12" s="27"/>
+      <c r="IX12" s="27"/>
+      <c r="IY12" s="27"/>
+      <c r="IZ12" s="27"/>
+    </row>
+    <row r="13" spans="1:260" s="1" customFormat="1" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="28" t="s">
         <v>113</v>
       </c>
       <c r="B13" s="10" t="s">
@@ -3872,13 +4224,13 @@
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
-      <c r="H13" s="9" t="s">
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="I13" s="27"/>
-      <c r="J13" s="27"/>
-      <c r="K13" s="27"/>
-      <c r="L13" s="27"/>
       <c r="M13" s="27"/>
       <c r="N13" s="27"/>
       <c r="O13" s="27"/>
@@ -4123,8 +4475,12 @@
       <c r="IT13" s="27"/>
       <c r="IU13" s="27"/>
       <c r="IV13" s="27"/>
-    </row>
-    <row r="14" spans="1:256" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="IW13" s="27"/>
+      <c r="IX13" s="27"/>
+      <c r="IY13" s="27"/>
+      <c r="IZ13" s="27"/>
+    </row>
+    <row r="14" spans="1:260" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="11"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
@@ -4133,8 +4489,12 @@
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
-    </row>
-    <row r="15" spans="1:256" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+    </row>
+    <row r="15" spans="1:260" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
         <v>15</v>
       </c>
@@ -4147,8 +4507,12 @@
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>
-    </row>
-    <row r="16" spans="1:256" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+    </row>
+    <row r="16" spans="1:260" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>17</v>
       </c>
@@ -4161,8 +4525,12 @@
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
       <c r="H16" s="10"/>
-    </row>
-    <row r="17" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+    </row>
+    <row r="17" spans="1:12" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="s">
         <v>19</v>
       </c>
@@ -4175,8 +4543,12 @@
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
-    </row>
-    <row r="18" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+    </row>
+    <row r="18" spans="1:12" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
         <v>21</v>
       </c>
@@ -4189,8 +4561,12 @@
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
       <c r="H18" s="10"/>
-    </row>
-    <row r="19" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+    </row>
+    <row r="19" spans="1:12" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="11"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
@@ -4199,8 +4575,12 @@
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
-    </row>
-    <row r="20" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+    </row>
+    <row r="20" spans="1:12" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="14"/>
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
@@ -4209,8 +4589,12 @@
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
       <c r="H20" s="10"/>
-    </row>
-    <row r="21" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+    </row>
+    <row r="21" spans="1:12" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="14"/>
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
@@ -4219,8 +4603,12 @@
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
-    </row>
-    <row r="22" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+    </row>
+    <row r="22" spans="1:12" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="14"/>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
@@ -4229,8 +4617,12 @@
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
       <c r="H22" s="10"/>
-    </row>
-    <row r="23" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+    </row>
+    <row r="23" spans="1:12" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="15" t="s">
         <v>23</v>
       </c>
@@ -4246,11 +4638,15 @@
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
-      <c r="H23" s="16" t="s">
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="16" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="s">
         <v>27</v>
       </c>
@@ -4272,11 +4668,15 @@
       <c r="G24" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="H24" s="9" t="s">
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
         <v>34</v>
       </c>
@@ -4294,11 +4694,15 @@
       </c>
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
-      <c r="H25" s="9" t="s">
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
         <v>39</v>
       </c>
@@ -4314,11 +4718,15 @@
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
-      <c r="H26" s="9" t="s">
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="9" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="15" t="s">
         <v>43</v>
       </c>
@@ -4334,11 +4742,15 @@
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
-      <c r="H27" s="9" t="s">
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="9" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="11"/>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
@@ -4347,8 +4759,12 @@
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
       <c r="H28" s="10"/>
-    </row>
-    <row r="29" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+    </row>
+    <row r="29" spans="1:12" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="11"/>
       <c r="B29" s="9"/>
       <c r="C29" s="10"/>
@@ -4356,9 +4772,13 @@
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
-      <c r="H29" s="9"/>
-    </row>
-    <row r="30" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="9"/>
+    </row>
+    <row r="30" spans="1:12" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="11"/>
       <c r="B30" s="9"/>
       <c r="C30" s="10"/>
@@ -4366,9 +4786,13 @@
       <c r="E30" s="10"/>
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
-      <c r="H30" s="9"/>
-    </row>
-    <row r="31" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="9"/>
+    </row>
+    <row r="31" spans="1:12" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="11"/>
       <c r="B31" s="9"/>
       <c r="C31" s="10"/>
@@ -4376,9 +4800,13 @@
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
       <c r="G31" s="10"/>
-      <c r="H31" s="9"/>
-    </row>
-    <row r="32" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="9"/>
+    </row>
+    <row r="32" spans="1:12" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="18" t="s">
         <v>47</v>
       </c>
@@ -4394,11 +4822,15 @@
       <c r="E32" s="10"/>
       <c r="F32" s="10"/>
       <c r="G32" s="10"/>
-      <c r="H32" s="9" t="s">
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="10"/>
+      <c r="L32" s="9" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:260" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="18" t="s">
         <v>51</v>
       </c>
@@ -4414,11 +4846,15 @@
       <c r="E33" s="10"/>
       <c r="F33" s="10"/>
       <c r="G33" s="10"/>
-      <c r="H33" s="9" t="s">
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
+      <c r="L33" s="9" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:260" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="18" t="s">
         <v>54</v>
       </c>
@@ -4441,8 +4877,12 @@
         <v>59</v>
       </c>
       <c r="H34" s="9"/>
-    </row>
-    <row r="35" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I34" s="9"/>
+      <c r="J34" s="9"/>
+      <c r="K34" s="9"/>
+      <c r="L34" s="9"/>
+    </row>
+    <row r="35" spans="1:260" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="11"/>
       <c r="B35" s="9"/>
       <c r="C35" s="10"/>
@@ -4450,81 +4890,793 @@
       <c r="E35" s="10"/>
       <c r="F35" s="10"/>
       <c r="G35" s="10"/>
-      <c r="H35" s="9"/>
-    </row>
-    <row r="36" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="11"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="10"/>
+      <c r="K35" s="10"/>
+      <c r="L35" s="33"/>
+    </row>
+    <row r="36" spans="1:260" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="40" t="s">
+        <v>156</v>
+      </c>
       <c r="B36" s="9"/>
-      <c r="C36" s="10"/>
+      <c r="C36" s="10">
+        <v>8</v>
+      </c>
       <c r="D36" s="10"/>
       <c r="E36" s="10"/>
       <c r="F36" s="10"/>
       <c r="G36" s="10"/>
-      <c r="H36" s="9"/>
-    </row>
-    <row r="37" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="11"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="37"/>
+      <c r="L36" s="39" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="37" spans="1:260" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="40" t="s">
+        <v>157</v>
+      </c>
       <c r="B37" s="9"/>
-      <c r="C37" s="10"/>
+      <c r="C37" s="10">
+        <v>8</v>
+      </c>
       <c r="D37" s="10"/>
       <c r="E37" s="10"/>
       <c r="F37" s="10"/>
       <c r="G37" s="10"/>
-      <c r="H37" s="9"/>
-    </row>
-    <row r="38" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="11"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="10"/>
+      <c r="J37" s="10"/>
+      <c r="K37" s="37"/>
+      <c r="L37" s="39"/>
+    </row>
+    <row r="38" spans="1:260" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="40" t="s">
+        <v>158</v>
+      </c>
       <c r="B38" s="9"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="10"/>
-      <c r="G38" s="10"/>
-      <c r="H38" s="9"/>
-    </row>
-    <row r="39" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="11"/>
+      <c r="C38" s="10">
+        <v>6</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="F38" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="G38" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="H38" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="I38" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="J38" s="10"/>
+      <c r="K38" s="10"/>
+      <c r="L38" s="38"/>
+    </row>
+    <row r="39" spans="1:260" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="40" t="s">
+        <v>159</v>
+      </c>
       <c r="B39" s="9"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="9"/>
-    </row>
-    <row r="40" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="11"/>
+      <c r="C39" s="10">
+        <v>6</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="F39" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="G39" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="H39" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="I39" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="J39" s="10"/>
+      <c r="K39" s="10"/>
+      <c r="L39" s="9"/>
+    </row>
+    <row r="40" spans="1:260" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="40" t="s">
+        <v>160</v>
+      </c>
       <c r="B40" s="9"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="10"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="10"/>
-      <c r="G40" s="10"/>
-      <c r="H40" s="9"/>
-    </row>
-    <row r="41" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="11"/>
+      <c r="C40" s="10">
+        <v>6</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="F40" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="G40" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="H40" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="I40" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="J40" s="10"/>
+      <c r="K40" s="10"/>
+      <c r="L40" s="9"/>
+    </row>
+    <row r="41" spans="1:260" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="40" t="s">
+        <v>161</v>
+      </c>
       <c r="B41" s="9"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="10"/>
-      <c r="F41" s="10"/>
-      <c r="G41" s="10"/>
-      <c r="H41" s="9"/>
-    </row>
-    <row r="42" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="11"/>
-      <c r="B42" s="9"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="10"/>
-      <c r="G42" s="10"/>
-      <c r="H42" s="9"/>
+      <c r="C41" s="10">
+        <v>8</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="F41" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="G41" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="H41" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="I41" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="J41" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="K41" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="L41" s="9"/>
+    </row>
+    <row r="42" spans="1:260" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="41" t="s">
+        <v>162</v>
+      </c>
+      <c r="B42" s="33"/>
+      <c r="C42" s="34">
+        <v>6</v>
+      </c>
+      <c r="D42" s="34" t="s">
+        <v>147</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="F42" s="34" t="s">
+        <v>148</v>
+      </c>
+      <c r="G42" s="34" t="s">
+        <v>149</v>
+      </c>
+      <c r="H42" s="34" t="s">
+        <v>150</v>
+      </c>
+      <c r="I42" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="J42" s="34" t="s">
+        <v>152</v>
+      </c>
+      <c r="K42" s="34"/>
+      <c r="L42" s="33"/>
+    </row>
+    <row r="43" spans="1:260" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="42" t="s">
+        <v>163</v>
+      </c>
+      <c r="B43" s="43"/>
+      <c r="C43" s="43">
+        <v>6</v>
+      </c>
+      <c r="D43" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="E43" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="F43" s="43" t="s">
+        <v>165</v>
+      </c>
+      <c r="G43" s="43" t="s">
+        <v>166</v>
+      </c>
+      <c r="H43" s="43" t="s">
+        <v>167</v>
+      </c>
+      <c r="I43" s="43" t="s">
+        <v>168</v>
+      </c>
+      <c r="J43" s="43"/>
+      <c r="K43" s="43"/>
+      <c r="L43" s="43"/>
+    </row>
+    <row r="44" spans="1:260" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="36" t="s">
+        <v>164</v>
+      </c>
+      <c r="B44" s="35"/>
+      <c r="C44" s="35">
+        <v>6</v>
+      </c>
+      <c r="D44" s="35" t="s">
+        <v>169</v>
+      </c>
+      <c r="E44" s="35" t="s">
+        <v>170</v>
+      </c>
+      <c r="F44" s="35" t="s">
+        <v>171</v>
+      </c>
+      <c r="G44" s="35" t="s">
+        <v>172</v>
+      </c>
+      <c r="H44" s="35" t="s">
+        <v>173</v>
+      </c>
+      <c r="I44" s="35" t="s">
+        <v>174</v>
+      </c>
+      <c r="J44" s="35"/>
+      <c r="K44" s="35"/>
+      <c r="L44" s="35"/>
+    </row>
+    <row r="45" spans="1:260" s="46" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="44"/>
+      <c r="B45" s="45"/>
+      <c r="C45" s="45"/>
+      <c r="D45" s="45"/>
+      <c r="E45" s="45"/>
+      <c r="F45" s="45"/>
+      <c r="G45" s="45"/>
+      <c r="H45" s="45"/>
+      <c r="I45" s="45"/>
+      <c r="J45" s="45"/>
+      <c r="K45" s="45"/>
+      <c r="L45" s="45"/>
+      <c r="M45" s="45"/>
+      <c r="N45" s="45"/>
+      <c r="O45" s="45"/>
+      <c r="P45" s="45"/>
+      <c r="Q45" s="45"/>
+      <c r="R45" s="45"/>
+      <c r="S45" s="45"/>
+      <c r="T45" s="45"/>
+      <c r="U45" s="45"/>
+      <c r="V45" s="45"/>
+      <c r="W45" s="45"/>
+      <c r="X45" s="45"/>
+      <c r="Y45" s="45"/>
+      <c r="Z45" s="45"/>
+      <c r="AA45" s="45"/>
+      <c r="AB45" s="45"/>
+      <c r="AC45" s="45"/>
+      <c r="AD45" s="45"/>
+      <c r="AE45" s="45"/>
+      <c r="AF45" s="45"/>
+      <c r="AG45" s="45"/>
+      <c r="AH45" s="45"/>
+      <c r="AI45" s="45"/>
+      <c r="AJ45" s="45"/>
+      <c r="AK45" s="45"/>
+      <c r="AL45" s="45"/>
+      <c r="AM45" s="45"/>
+      <c r="AN45" s="45"/>
+      <c r="AO45" s="45"/>
+      <c r="AP45" s="45"/>
+      <c r="AQ45" s="45"/>
+      <c r="AR45" s="45"/>
+      <c r="AS45" s="45"/>
+      <c r="AT45" s="45"/>
+      <c r="AU45" s="45"/>
+      <c r="AV45" s="45"/>
+      <c r="AW45" s="45"/>
+      <c r="AX45" s="45"/>
+      <c r="AY45" s="45"/>
+      <c r="AZ45" s="45"/>
+      <c r="BA45" s="45"/>
+      <c r="BB45" s="45"/>
+      <c r="BC45" s="45"/>
+      <c r="BD45" s="45"/>
+      <c r="BE45" s="45"/>
+      <c r="BF45" s="45"/>
+      <c r="BG45" s="45"/>
+      <c r="BH45" s="45"/>
+      <c r="BI45" s="45"/>
+      <c r="BJ45" s="45"/>
+      <c r="BK45" s="45"/>
+      <c r="BL45" s="45"/>
+      <c r="BM45" s="45"/>
+      <c r="BN45" s="45"/>
+      <c r="BO45" s="45"/>
+      <c r="BP45" s="45"/>
+      <c r="BQ45" s="45"/>
+      <c r="BR45" s="45"/>
+      <c r="BS45" s="45"/>
+      <c r="BT45" s="45"/>
+      <c r="BU45" s="45"/>
+      <c r="BV45" s="45"/>
+      <c r="BW45" s="45"/>
+      <c r="BX45" s="45"/>
+      <c r="BY45" s="45"/>
+      <c r="BZ45" s="45"/>
+      <c r="CA45" s="45"/>
+      <c r="CB45" s="45"/>
+      <c r="CC45" s="45"/>
+      <c r="CD45" s="45"/>
+      <c r="CE45" s="45"/>
+      <c r="CF45" s="45"/>
+      <c r="CG45" s="45"/>
+      <c r="CH45" s="45"/>
+      <c r="CI45" s="45"/>
+      <c r="CJ45" s="45"/>
+      <c r="CK45" s="45"/>
+      <c r="CL45" s="45"/>
+      <c r="CM45" s="45"/>
+      <c r="CN45" s="45"/>
+      <c r="CO45" s="45"/>
+      <c r="CP45" s="45"/>
+      <c r="CQ45" s="45"/>
+      <c r="CR45" s="45"/>
+      <c r="CS45" s="45"/>
+      <c r="CT45" s="45"/>
+      <c r="CU45" s="45"/>
+      <c r="CV45" s="45"/>
+      <c r="CW45" s="45"/>
+      <c r="CX45" s="45"/>
+      <c r="CY45" s="45"/>
+      <c r="CZ45" s="45"/>
+      <c r="DA45" s="45"/>
+      <c r="DB45" s="45"/>
+      <c r="DC45" s="45"/>
+      <c r="DD45" s="45"/>
+      <c r="DE45" s="45"/>
+      <c r="DF45" s="45"/>
+      <c r="DG45" s="45"/>
+      <c r="DH45" s="45"/>
+      <c r="DI45" s="45"/>
+      <c r="DJ45" s="45"/>
+      <c r="DK45" s="45"/>
+      <c r="DL45" s="45"/>
+      <c r="DM45" s="45"/>
+      <c r="DN45" s="45"/>
+      <c r="DO45" s="45"/>
+      <c r="DP45" s="45"/>
+      <c r="DQ45" s="45"/>
+      <c r="DR45" s="45"/>
+      <c r="DS45" s="45"/>
+      <c r="DT45" s="45"/>
+      <c r="DU45" s="45"/>
+      <c r="DV45" s="45"/>
+      <c r="DW45" s="45"/>
+      <c r="DX45" s="45"/>
+      <c r="DY45" s="45"/>
+      <c r="DZ45" s="45"/>
+      <c r="EA45" s="45"/>
+      <c r="EB45" s="45"/>
+      <c r="EC45" s="45"/>
+      <c r="ED45" s="45"/>
+      <c r="EE45" s="45"/>
+      <c r="EF45" s="45"/>
+      <c r="EG45" s="45"/>
+      <c r="EH45" s="45"/>
+      <c r="EI45" s="45"/>
+      <c r="EJ45" s="45"/>
+      <c r="EK45" s="45"/>
+      <c r="EL45" s="45"/>
+      <c r="EM45" s="45"/>
+      <c r="EN45" s="45"/>
+      <c r="EO45" s="45"/>
+      <c r="EP45" s="45"/>
+      <c r="EQ45" s="45"/>
+      <c r="ER45" s="45"/>
+      <c r="ES45" s="45"/>
+      <c r="ET45" s="45"/>
+      <c r="EU45" s="45"/>
+      <c r="EV45" s="45"/>
+      <c r="EW45" s="45"/>
+      <c r="EX45" s="45"/>
+      <c r="EY45" s="45"/>
+      <c r="EZ45" s="45"/>
+      <c r="FA45" s="45"/>
+      <c r="FB45" s="45"/>
+      <c r="FC45" s="45"/>
+      <c r="FD45" s="45"/>
+      <c r="FE45" s="45"/>
+      <c r="FF45" s="45"/>
+      <c r="FG45" s="45"/>
+      <c r="FH45" s="45"/>
+      <c r="FI45" s="45"/>
+      <c r="FJ45" s="45"/>
+      <c r="FK45" s="45"/>
+      <c r="FL45" s="45"/>
+      <c r="FM45" s="45"/>
+      <c r="FN45" s="45"/>
+      <c r="FO45" s="45"/>
+      <c r="FP45" s="45"/>
+      <c r="FQ45" s="45"/>
+      <c r="FR45" s="45"/>
+      <c r="FS45" s="45"/>
+      <c r="FT45" s="45"/>
+      <c r="FU45" s="45"/>
+      <c r="FV45" s="45"/>
+      <c r="FW45" s="45"/>
+      <c r="FX45" s="45"/>
+      <c r="FY45" s="45"/>
+      <c r="FZ45" s="45"/>
+      <c r="GA45" s="45"/>
+      <c r="GB45" s="45"/>
+      <c r="GC45" s="45"/>
+      <c r="GD45" s="45"/>
+      <c r="GE45" s="45"/>
+      <c r="GF45" s="45"/>
+      <c r="GG45" s="45"/>
+      <c r="GH45" s="45"/>
+      <c r="GI45" s="45"/>
+      <c r="GJ45" s="45"/>
+      <c r="GK45" s="45"/>
+      <c r="GL45" s="45"/>
+      <c r="GM45" s="45"/>
+      <c r="GN45" s="45"/>
+      <c r="GO45" s="45"/>
+      <c r="GP45" s="45"/>
+      <c r="GQ45" s="45"/>
+      <c r="GR45" s="45"/>
+      <c r="GS45" s="45"/>
+      <c r="GT45" s="45"/>
+      <c r="GU45" s="45"/>
+      <c r="GV45" s="45"/>
+      <c r="GW45" s="45"/>
+      <c r="GX45" s="45"/>
+      <c r="GY45" s="45"/>
+      <c r="GZ45" s="45"/>
+      <c r="HA45" s="45"/>
+      <c r="HB45" s="45"/>
+      <c r="HC45" s="45"/>
+      <c r="HD45" s="45"/>
+      <c r="HE45" s="45"/>
+      <c r="HF45" s="45"/>
+      <c r="HG45" s="45"/>
+      <c r="HH45" s="45"/>
+      <c r="HI45" s="45"/>
+      <c r="HJ45" s="45"/>
+      <c r="HK45" s="45"/>
+      <c r="HL45" s="45"/>
+      <c r="HM45" s="45"/>
+      <c r="HN45" s="45"/>
+      <c r="HO45" s="45"/>
+      <c r="HP45" s="45"/>
+      <c r="HQ45" s="45"/>
+      <c r="HR45" s="45"/>
+      <c r="HS45" s="45"/>
+      <c r="HT45" s="45"/>
+      <c r="HU45" s="45"/>
+      <c r="HV45" s="45"/>
+      <c r="HW45" s="45"/>
+      <c r="HX45" s="45"/>
+      <c r="HY45" s="45"/>
+      <c r="HZ45" s="45"/>
+      <c r="IA45" s="45"/>
+      <c r="IB45" s="45"/>
+      <c r="IC45" s="45"/>
+      <c r="ID45" s="45"/>
+      <c r="IE45" s="45"/>
+      <c r="IF45" s="45"/>
+      <c r="IG45" s="45"/>
+      <c r="IH45" s="45"/>
+      <c r="II45" s="45"/>
+      <c r="IJ45" s="45"/>
+      <c r="IK45" s="45"/>
+      <c r="IL45" s="45"/>
+      <c r="IM45" s="45"/>
+      <c r="IN45" s="45"/>
+      <c r="IO45" s="45"/>
+      <c r="IP45" s="45"/>
+      <c r="IQ45" s="45"/>
+      <c r="IR45" s="45"/>
+      <c r="IS45" s="45"/>
+      <c r="IT45" s="45"/>
+      <c r="IU45" s="45"/>
+      <c r="IV45" s="45"/>
+      <c r="IW45" s="45"/>
+      <c r="IX45" s="45"/>
+      <c r="IY45" s="45"/>
+      <c r="IZ45" s="45"/>
+    </row>
+    <row r="46" spans="1:260" s="46" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="44"/>
+      <c r="B46" s="45"/>
+      <c r="C46" s="45"/>
+      <c r="D46" s="45"/>
+      <c r="E46" s="45"/>
+      <c r="F46" s="45"/>
+      <c r="G46" s="45"/>
+      <c r="H46" s="45"/>
+      <c r="I46" s="45"/>
+      <c r="J46" s="45"/>
+      <c r="K46" s="45"/>
+      <c r="L46" s="45"/>
+      <c r="M46" s="45"/>
+      <c r="N46" s="45"/>
+      <c r="O46" s="45"/>
+      <c r="P46" s="45"/>
+      <c r="Q46" s="45"/>
+      <c r="R46" s="45"/>
+      <c r="S46" s="45"/>
+      <c r="T46" s="45"/>
+      <c r="U46" s="45"/>
+      <c r="V46" s="45"/>
+      <c r="W46" s="45"/>
+      <c r="X46" s="45"/>
+      <c r="Y46" s="45"/>
+      <c r="Z46" s="45"/>
+      <c r="AA46" s="45"/>
+      <c r="AB46" s="45"/>
+      <c r="AC46" s="45"/>
+      <c r="AD46" s="45"/>
+      <c r="AE46" s="45"/>
+      <c r="AF46" s="45"/>
+      <c r="AG46" s="45"/>
+      <c r="AH46" s="45"/>
+      <c r="AI46" s="45"/>
+      <c r="AJ46" s="45"/>
+      <c r="AK46" s="45"/>
+      <c r="AL46" s="45"/>
+      <c r="AM46" s="45"/>
+      <c r="AN46" s="45"/>
+      <c r="AO46" s="45"/>
+      <c r="AP46" s="45"/>
+      <c r="AQ46" s="45"/>
+      <c r="AR46" s="45"/>
+      <c r="AS46" s="45"/>
+      <c r="AT46" s="45"/>
+      <c r="AU46" s="45"/>
+      <c r="AV46" s="45"/>
+      <c r="AW46" s="45"/>
+      <c r="AX46" s="45"/>
+      <c r="AY46" s="45"/>
+      <c r="AZ46" s="45"/>
+      <c r="BA46" s="45"/>
+      <c r="BB46" s="45"/>
+      <c r="BC46" s="45"/>
+      <c r="BD46" s="45"/>
+      <c r="BE46" s="45"/>
+      <c r="BF46" s="45"/>
+      <c r="BG46" s="45"/>
+      <c r="BH46" s="45"/>
+      <c r="BI46" s="45"/>
+      <c r="BJ46" s="45"/>
+      <c r="BK46" s="45"/>
+      <c r="BL46" s="45"/>
+      <c r="BM46" s="45"/>
+      <c r="BN46" s="45"/>
+      <c r="BO46" s="45"/>
+      <c r="BP46" s="45"/>
+      <c r="BQ46" s="45"/>
+      <c r="BR46" s="45"/>
+      <c r="BS46" s="45"/>
+      <c r="BT46" s="45"/>
+      <c r="BU46" s="45"/>
+      <c r="BV46" s="45"/>
+      <c r="BW46" s="45"/>
+      <c r="BX46" s="45"/>
+      <c r="BY46" s="45"/>
+      <c r="BZ46" s="45"/>
+      <c r="CA46" s="45"/>
+      <c r="CB46" s="45"/>
+      <c r="CC46" s="45"/>
+      <c r="CD46" s="45"/>
+      <c r="CE46" s="45"/>
+      <c r="CF46" s="45"/>
+      <c r="CG46" s="45"/>
+      <c r="CH46" s="45"/>
+      <c r="CI46" s="45"/>
+      <c r="CJ46" s="45"/>
+      <c r="CK46" s="45"/>
+      <c r="CL46" s="45"/>
+      <c r="CM46" s="45"/>
+      <c r="CN46" s="45"/>
+      <c r="CO46" s="45"/>
+      <c r="CP46" s="45"/>
+      <c r="CQ46" s="45"/>
+      <c r="CR46" s="45"/>
+      <c r="CS46" s="45"/>
+      <c r="CT46" s="45"/>
+      <c r="CU46" s="45"/>
+      <c r="CV46" s="45"/>
+      <c r="CW46" s="45"/>
+      <c r="CX46" s="45"/>
+      <c r="CY46" s="45"/>
+      <c r="CZ46" s="45"/>
+      <c r="DA46" s="45"/>
+      <c r="DB46" s="45"/>
+      <c r="DC46" s="45"/>
+      <c r="DD46" s="45"/>
+      <c r="DE46" s="45"/>
+      <c r="DF46" s="45"/>
+      <c r="DG46" s="45"/>
+      <c r="DH46" s="45"/>
+      <c r="DI46" s="45"/>
+      <c r="DJ46" s="45"/>
+      <c r="DK46" s="45"/>
+      <c r="DL46" s="45"/>
+      <c r="DM46" s="45"/>
+      <c r="DN46" s="45"/>
+      <c r="DO46" s="45"/>
+      <c r="DP46" s="45"/>
+      <c r="DQ46" s="45"/>
+      <c r="DR46" s="45"/>
+      <c r="DS46" s="45"/>
+      <c r="DT46" s="45"/>
+      <c r="DU46" s="45"/>
+      <c r="DV46" s="45"/>
+      <c r="DW46" s="45"/>
+      <c r="DX46" s="45"/>
+      <c r="DY46" s="45"/>
+      <c r="DZ46" s="45"/>
+      <c r="EA46" s="45"/>
+      <c r="EB46" s="45"/>
+      <c r="EC46" s="45"/>
+      <c r="ED46" s="45"/>
+      <c r="EE46" s="45"/>
+      <c r="EF46" s="45"/>
+      <c r="EG46" s="45"/>
+      <c r="EH46" s="45"/>
+      <c r="EI46" s="45"/>
+      <c r="EJ46" s="45"/>
+      <c r="EK46" s="45"/>
+      <c r="EL46" s="45"/>
+      <c r="EM46" s="45"/>
+      <c r="EN46" s="45"/>
+      <c r="EO46" s="45"/>
+      <c r="EP46" s="45"/>
+      <c r="EQ46" s="45"/>
+      <c r="ER46" s="45"/>
+      <c r="ES46" s="45"/>
+      <c r="ET46" s="45"/>
+      <c r="EU46" s="45"/>
+      <c r="EV46" s="45"/>
+      <c r="EW46" s="45"/>
+      <c r="EX46" s="45"/>
+      <c r="EY46" s="45"/>
+      <c r="EZ46" s="45"/>
+      <c r="FA46" s="45"/>
+      <c r="FB46" s="45"/>
+      <c r="FC46" s="45"/>
+      <c r="FD46" s="45"/>
+      <c r="FE46" s="45"/>
+      <c r="FF46" s="45"/>
+      <c r="FG46" s="45"/>
+      <c r="FH46" s="45"/>
+      <c r="FI46" s="45"/>
+      <c r="FJ46" s="45"/>
+      <c r="FK46" s="45"/>
+      <c r="FL46" s="45"/>
+      <c r="FM46" s="45"/>
+      <c r="FN46" s="45"/>
+      <c r="FO46" s="45"/>
+      <c r="FP46" s="45"/>
+      <c r="FQ46" s="45"/>
+      <c r="FR46" s="45"/>
+      <c r="FS46" s="45"/>
+      <c r="FT46" s="45"/>
+      <c r="FU46" s="45"/>
+      <c r="FV46" s="45"/>
+      <c r="FW46" s="45"/>
+      <c r="FX46" s="45"/>
+      <c r="FY46" s="45"/>
+      <c r="FZ46" s="45"/>
+      <c r="GA46" s="45"/>
+      <c r="GB46" s="45"/>
+      <c r="GC46" s="45"/>
+      <c r="GD46" s="45"/>
+      <c r="GE46" s="45"/>
+      <c r="GF46" s="45"/>
+      <c r="GG46" s="45"/>
+      <c r="GH46" s="45"/>
+      <c r="GI46" s="45"/>
+      <c r="GJ46" s="45"/>
+      <c r="GK46" s="45"/>
+      <c r="GL46" s="45"/>
+      <c r="GM46" s="45"/>
+      <c r="GN46" s="45"/>
+      <c r="GO46" s="45"/>
+      <c r="GP46" s="45"/>
+      <c r="GQ46" s="45"/>
+      <c r="GR46" s="45"/>
+      <c r="GS46" s="45"/>
+      <c r="GT46" s="45"/>
+      <c r="GU46" s="45"/>
+      <c r="GV46" s="45"/>
+      <c r="GW46" s="45"/>
+      <c r="GX46" s="45"/>
+      <c r="GY46" s="45"/>
+      <c r="GZ46" s="45"/>
+      <c r="HA46" s="45"/>
+      <c r="HB46" s="45"/>
+      <c r="HC46" s="45"/>
+      <c r="HD46" s="45"/>
+      <c r="HE46" s="45"/>
+      <c r="HF46" s="45"/>
+      <c r="HG46" s="45"/>
+      <c r="HH46" s="45"/>
+      <c r="HI46" s="45"/>
+      <c r="HJ46" s="45"/>
+      <c r="HK46" s="45"/>
+      <c r="HL46" s="45"/>
+      <c r="HM46" s="45"/>
+      <c r="HN46" s="45"/>
+      <c r="HO46" s="45"/>
+      <c r="HP46" s="45"/>
+      <c r="HQ46" s="45"/>
+      <c r="HR46" s="45"/>
+      <c r="HS46" s="45"/>
+      <c r="HT46" s="45"/>
+      <c r="HU46" s="45"/>
+      <c r="HV46" s="45"/>
+      <c r="HW46" s="45"/>
+      <c r="HX46" s="45"/>
+      <c r="HY46" s="45"/>
+      <c r="HZ46" s="45"/>
+      <c r="IA46" s="45"/>
+      <c r="IB46" s="45"/>
+      <c r="IC46" s="45"/>
+      <c r="ID46" s="45"/>
+      <c r="IE46" s="45"/>
+      <c r="IF46" s="45"/>
+      <c r="IG46" s="45"/>
+      <c r="IH46" s="45"/>
+      <c r="II46" s="45"/>
+      <c r="IJ46" s="45"/>
+      <c r="IK46" s="45"/>
+      <c r="IL46" s="45"/>
+      <c r="IM46" s="45"/>
+      <c r="IN46" s="45"/>
+      <c r="IO46" s="45"/>
+      <c r="IP46" s="45"/>
+      <c r="IQ46" s="45"/>
+      <c r="IR46" s="45"/>
+      <c r="IS46" s="45"/>
+      <c r="IT46" s="45"/>
+      <c r="IU46" s="45"/>
+      <c r="IV46" s="45"/>
+      <c r="IW46" s="45"/>
+      <c r="IX46" s="45"/>
+      <c r="IY46" s="45"/>
+      <c r="IZ46" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A1:L1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4539,9 +5691,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IV6"/>
+  <dimension ref="A1:IV7"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.19921875" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4576,6 +5730,11 @@
     <row r="6" spans="1:1" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
         <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="32" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -4609,10 +5768,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="28"/>
+      <c r="B1" s="30"/>
     </row>
     <row r="2" spans="1:2" ht="20.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
@@ -4704,17 +5863,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
     </row>
     <row r="2" spans="1:9" ht="20.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">

</xml_diff>

<commit_message>
modifies names and added messages
</commit_message>
<xml_diff>
--- a/ION CAN Messages.xlsx
+++ b/ION CAN Messages.xlsx
@@ -5,11 +5,11 @@
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sindre\Documents\GitHub\Dokumentasjon\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Morten\Documents\GitHub\Dokumentasjon\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="7710" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Export Summary" sheetId="1" r:id="rId1"/>
@@ -17,14 +17,15 @@
     <sheet name="ID List - Table 1" sheetId="3" r:id="rId3"/>
     <sheet name="1_ Pedalmodul - CAN_MSG_PEDALS_" sheetId="4" r:id="rId4"/>
     <sheet name="1_ Pedalmodul - CAN_MSG_PEDALS1" sheetId="5" r:id="rId5"/>
-    <sheet name="1_ Pedalmodul - Drawings" sheetId="6" r:id="rId6"/>
+    <sheet name="Ark1" sheetId="7" r:id="rId6"/>
+    <sheet name="1_ Pedalmodul - Drawings" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="223">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -110,9 +111,6 @@
     <t>0x310</t>
   </si>
   <si>
-    <t>CAN_MSG_PEDALS</t>
-  </si>
-  <si>
     <t>TORQUE[16:8]</t>
   </si>
   <si>
@@ -125,9 +123,6 @@
     <t>BRAKE[8:0]</t>
   </si>
   <si>
-    <t>Torque- &amp; brake-encoder values (12-bit values; 0xFFF max, 0x000 min)</t>
-  </si>
-  <si>
     <t>0x311</t>
   </si>
   <si>
@@ -152,9 +147,6 @@
     <t>CALIBRATION[8:0]</t>
   </si>
   <si>
-    <t>Start calibration (pedals / steering, see sheet 1)</t>
-  </si>
-  <si>
     <t>0x321</t>
   </si>
   <si>
@@ -311,9 +303,6 @@
     <t>CAN_MSG_PRECHARGE</t>
   </si>
   <si>
-    <t>CAN_MSG_CURRENT_SENSOR</t>
-  </si>
-  <si>
     <t>CAN_MSG_HV_SENSOR</t>
   </si>
   <si>
@@ -371,9 +360,6 @@
     <t>CAN_MSG_CURRENT_SENSOR_CALIBRATE</t>
   </si>
   <si>
-    <t>Current sensor value</t>
-  </si>
-  <si>
     <t>Hv sensor value</t>
   </si>
   <si>
@@ -552,6 +538,162 @@
   </si>
   <si>
     <t>Descriptions: http://lithiumate.elithion.com/php/controller_can_specs.php</t>
+  </si>
+  <si>
+    <t>0x004</t>
+  </si>
+  <si>
+    <t>CAN_MSG_OVERCURRENT</t>
+  </si>
+  <si>
+    <t>CURRENT[8:0]</t>
+  </si>
+  <si>
+    <t>Sent if OVERCURRENT.</t>
+  </si>
+  <si>
+    <t>HV[16:8]</t>
+  </si>
+  <si>
+    <t>HV[8:0]</t>
+  </si>
+  <si>
+    <t>LV[8:0]</t>
+  </si>
+  <si>
+    <t>LV[16:8]</t>
+  </si>
+  <si>
+    <t>CAN_MSG_CURRENT_SENSOR_AND_POWER</t>
+  </si>
+  <si>
+    <t>POWER[16:8]</t>
+  </si>
+  <si>
+    <t>POWER[8:0]</t>
+  </si>
+  <si>
+    <t>POWER[24:16]</t>
+  </si>
+  <si>
+    <t>0x451</t>
+  </si>
+  <si>
+    <t>CAN_MSG_WHEEL_RPM_REAR</t>
+  </si>
+  <si>
+    <t>CAN_MSG_PEDALS_STEERING</t>
+  </si>
+  <si>
+    <t>CAN_MSG_PEDALS_MIN_CALIBRATE</t>
+  </si>
+  <si>
+    <t>CAN_MSG_PEDALS_MIN_CALIBRATION_COMPLETE</t>
+  </si>
+  <si>
+    <t>CAN_MSG_PEDALS_MAX_TORQUE_CALIBRATE</t>
+  </si>
+  <si>
+    <t>CAN_MSG_PEDALS_MAX_TORQUE_CAlLIBRATION_COMPLETE</t>
+  </si>
+  <si>
+    <t>0x322</t>
+  </si>
+  <si>
+    <t>0x323</t>
+  </si>
+  <si>
+    <t>Start calibration  min value (pedals / steering, see sheet 1)</t>
+  </si>
+  <si>
+    <t>Start calibration max value torque (pedals / steering, see sheet 1)</t>
+  </si>
+  <si>
+    <t>0x324</t>
+  </si>
+  <si>
+    <t>CAN_MSG_PEDALS_MAX_BRAKE_CALIBRATE</t>
+  </si>
+  <si>
+    <t>CAN_MSG_PEDALS_MAX_BRAKE_CAlLIBRATION_COMPLETE</t>
+  </si>
+  <si>
+    <t>CAN_MSG_PEDALS_LEFT_STEERING_CALIBRATION_COMPLETE</t>
+  </si>
+  <si>
+    <t>0x325</t>
+  </si>
+  <si>
+    <t>0x326</t>
+  </si>
+  <si>
+    <t>0x327</t>
+  </si>
+  <si>
+    <t>0x328</t>
+  </si>
+  <si>
+    <t>0x329</t>
+  </si>
+  <si>
+    <t>0x330</t>
+  </si>
+  <si>
+    <t>CAN_MSG_PEDALS_LEFT_STEERING_CALIBRATE</t>
+  </si>
+  <si>
+    <t>CAN_MSG_PEDALS_CENTER_STEERING_CALIBRATE</t>
+  </si>
+  <si>
+    <t>CAN_MSG_PEDALS_CENTER_STEERING_CALIBRATION_COMPLETE</t>
+  </si>
+  <si>
+    <t>CAN_MSG_PEDALS_RIGHT_STEERING_CALIBRATE</t>
+  </si>
+  <si>
+    <t>CAN_MSG_PEDALS_RIGHT_STEERING_CALIBRATION_COMPLETE</t>
+  </si>
+  <si>
+    <t>Left steering calibration</t>
+  </si>
+  <si>
+    <t>Center steering calibration</t>
+  </si>
+  <si>
+    <t>Right steering calibration</t>
+  </si>
+  <si>
+    <t>Right steering calibration complete</t>
+  </si>
+  <si>
+    <t>Center steering calibration complete</t>
+  </si>
+  <si>
+    <t>Left steering calibration complete</t>
+  </si>
+  <si>
+    <t>Torque- &amp; brake-encoder values (15-bit values; 0x7FFF max, 0x0000 min)</t>
+  </si>
+  <si>
+    <t>0x331</t>
+  </si>
+  <si>
+    <t>0x332</t>
+  </si>
+  <si>
+    <t>CAN_MSG_PEDALS_AND_STEERING_CALIBRATION_COMPLETE</t>
+  </si>
+  <si>
+    <t>All sensors calibrated</t>
+  </si>
+  <si>
+    <t>STEERINGDIRECTION</t>
+  </si>
+  <si>
+    <t>powerDirection[8:0]</t>
+  </si>
+  <si>
+    <t>PowerDirection = 1 -&gt; from batt to motor, 0 -&gt; from motor to batt, Power and Current sensor value</t>
   </si>
 </sst>
 </file>
@@ -791,7 +933,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -877,9 +1019,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -923,6 +1062,15 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1046,7 +1194,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-            <ma14:wrappingTextBoxFlag xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+            <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" val="1"/>
           </a:ext>
         </a:extLst>
       </xdr:spPr>
@@ -2340,7 +2488,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:D15"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="12.95" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2349,11 +2499,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
     </row>
     <row r="7" spans="2:4" ht="18" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
@@ -2385,15 +2535,15 @@
     <row r="11" spans="2:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B11" s="4"/>
       <c r="C11" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -2401,28 +2551,28 @@
     <row r="13" spans="2:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B13" s="4"/>
       <c r="C13" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B14" s="4"/>
       <c r="C14" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B15" s="4"/>
       <c r="C15" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -2445,13 +2595,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IZ46"/>
+  <dimension ref="A1:IZ58"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="E31" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M38" sqref="M38"/>
+      <selection pane="bottomRight" activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2467,20 +2617,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:260" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
     </row>
     <row r="2" spans="1:260" ht="20.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
@@ -2546,10 +2696,10 @@
     </row>
     <row r="4" spans="1:260" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="28" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -2561,15 +2711,15 @@
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
       <c r="L4" s="9" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:260" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="28" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
@@ -2581,15 +2731,15 @@
       <c r="J5" s="10"/>
       <c r="K5" s="10"/>
       <c r="L5" s="9" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="6" spans="1:260" s="1" customFormat="1" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:260" s="30" customFormat="1" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="28" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
@@ -2601,7 +2751,7 @@
       <c r="J6" s="10"/>
       <c r="K6" s="10"/>
       <c r="L6" s="9" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="M6" s="27"/>
       <c r="N6" s="27"/>
@@ -2852,15 +3002,19 @@
       <c r="IY6" s="27"/>
       <c r="IZ6" s="27"/>
     </row>
-    <row r="7" spans="1:260" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:260" s="1" customFormat="1" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="28" t="s">
-        <v>102</v>
+        <v>171</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
+        <v>172</v>
+      </c>
+      <c r="C7" s="10">
+        <v>1</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>173</v>
+      </c>
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
@@ -2869,15 +3023,263 @@
       <c r="J7" s="10"/>
       <c r="K7" s="10"/>
       <c r="L7" s="9" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="8" spans="1:260" s="1" customFormat="1" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+        <v>174</v>
+      </c>
+      <c r="M7" s="27"/>
+      <c r="N7" s="27"/>
+      <c r="O7" s="27"/>
+      <c r="P7" s="27"/>
+      <c r="Q7" s="27"/>
+      <c r="R7" s="27"/>
+      <c r="S7" s="27"/>
+      <c r="T7" s="27"/>
+      <c r="U7" s="27"/>
+      <c r="V7" s="27"/>
+      <c r="W7" s="27"/>
+      <c r="X7" s="27"/>
+      <c r="Y7" s="27"/>
+      <c r="Z7" s="27"/>
+      <c r="AA7" s="27"/>
+      <c r="AB7" s="27"/>
+      <c r="AC7" s="27"/>
+      <c r="AD7" s="27"/>
+      <c r="AE7" s="27"/>
+      <c r="AF7" s="27"/>
+      <c r="AG7" s="27"/>
+      <c r="AH7" s="27"/>
+      <c r="AI7" s="27"/>
+      <c r="AJ7" s="27"/>
+      <c r="AK7" s="27"/>
+      <c r="AL7" s="27"/>
+      <c r="AM7" s="27"/>
+      <c r="AN7" s="27"/>
+      <c r="AO7" s="27"/>
+      <c r="AP7" s="27"/>
+      <c r="AQ7" s="27"/>
+      <c r="AR7" s="27"/>
+      <c r="AS7" s="27"/>
+      <c r="AT7" s="27"/>
+      <c r="AU7" s="27"/>
+      <c r="AV7" s="27"/>
+      <c r="AW7" s="27"/>
+      <c r="AX7" s="27"/>
+      <c r="AY7" s="27"/>
+      <c r="AZ7" s="27"/>
+      <c r="BA7" s="27"/>
+      <c r="BB7" s="27"/>
+      <c r="BC7" s="27"/>
+      <c r="BD7" s="27"/>
+      <c r="BE7" s="27"/>
+      <c r="BF7" s="27"/>
+      <c r="BG7" s="27"/>
+      <c r="BH7" s="27"/>
+      <c r="BI7" s="27"/>
+      <c r="BJ7" s="27"/>
+      <c r="BK7" s="27"/>
+      <c r="BL7" s="27"/>
+      <c r="BM7" s="27"/>
+      <c r="BN7" s="27"/>
+      <c r="BO7" s="27"/>
+      <c r="BP7" s="27"/>
+      <c r="BQ7" s="27"/>
+      <c r="BR7" s="27"/>
+      <c r="BS7" s="27"/>
+      <c r="BT7" s="27"/>
+      <c r="BU7" s="27"/>
+      <c r="BV7" s="27"/>
+      <c r="BW7" s="27"/>
+      <c r="BX7" s="27"/>
+      <c r="BY7" s="27"/>
+      <c r="BZ7" s="27"/>
+      <c r="CA7" s="27"/>
+      <c r="CB7" s="27"/>
+      <c r="CC7" s="27"/>
+      <c r="CD7" s="27"/>
+      <c r="CE7" s="27"/>
+      <c r="CF7" s="27"/>
+      <c r="CG7" s="27"/>
+      <c r="CH7" s="27"/>
+      <c r="CI7" s="27"/>
+      <c r="CJ7" s="27"/>
+      <c r="CK7" s="27"/>
+      <c r="CL7" s="27"/>
+      <c r="CM7" s="27"/>
+      <c r="CN7" s="27"/>
+      <c r="CO7" s="27"/>
+      <c r="CP7" s="27"/>
+      <c r="CQ7" s="27"/>
+      <c r="CR7" s="27"/>
+      <c r="CS7" s="27"/>
+      <c r="CT7" s="27"/>
+      <c r="CU7" s="27"/>
+      <c r="CV7" s="27"/>
+      <c r="CW7" s="27"/>
+      <c r="CX7" s="27"/>
+      <c r="CY7" s="27"/>
+      <c r="CZ7" s="27"/>
+      <c r="DA7" s="27"/>
+      <c r="DB7" s="27"/>
+      <c r="DC7" s="27"/>
+      <c r="DD7" s="27"/>
+      <c r="DE7" s="27"/>
+      <c r="DF7" s="27"/>
+      <c r="DG7" s="27"/>
+      <c r="DH7" s="27"/>
+      <c r="DI7" s="27"/>
+      <c r="DJ7" s="27"/>
+      <c r="DK7" s="27"/>
+      <c r="DL7" s="27"/>
+      <c r="DM7" s="27"/>
+      <c r="DN7" s="27"/>
+      <c r="DO7" s="27"/>
+      <c r="DP7" s="27"/>
+      <c r="DQ7" s="27"/>
+      <c r="DR7" s="27"/>
+      <c r="DS7" s="27"/>
+      <c r="DT7" s="27"/>
+      <c r="DU7" s="27"/>
+      <c r="DV7" s="27"/>
+      <c r="DW7" s="27"/>
+      <c r="DX7" s="27"/>
+      <c r="DY7" s="27"/>
+      <c r="DZ7" s="27"/>
+      <c r="EA7" s="27"/>
+      <c r="EB7" s="27"/>
+      <c r="EC7" s="27"/>
+      <c r="ED7" s="27"/>
+      <c r="EE7" s="27"/>
+      <c r="EF7" s="27"/>
+      <c r="EG7" s="27"/>
+      <c r="EH7" s="27"/>
+      <c r="EI7" s="27"/>
+      <c r="EJ7" s="27"/>
+      <c r="EK7" s="27"/>
+      <c r="EL7" s="27"/>
+      <c r="EM7" s="27"/>
+      <c r="EN7" s="27"/>
+      <c r="EO7" s="27"/>
+      <c r="EP7" s="27"/>
+      <c r="EQ7" s="27"/>
+      <c r="ER7" s="27"/>
+      <c r="ES7" s="27"/>
+      <c r="ET7" s="27"/>
+      <c r="EU7" s="27"/>
+      <c r="EV7" s="27"/>
+      <c r="EW7" s="27"/>
+      <c r="EX7" s="27"/>
+      <c r="EY7" s="27"/>
+      <c r="EZ7" s="27"/>
+      <c r="FA7" s="27"/>
+      <c r="FB7" s="27"/>
+      <c r="FC7" s="27"/>
+      <c r="FD7" s="27"/>
+      <c r="FE7" s="27"/>
+      <c r="FF7" s="27"/>
+      <c r="FG7" s="27"/>
+      <c r="FH7" s="27"/>
+      <c r="FI7" s="27"/>
+      <c r="FJ7" s="27"/>
+      <c r="FK7" s="27"/>
+      <c r="FL7" s="27"/>
+      <c r="FM7" s="27"/>
+      <c r="FN7" s="27"/>
+      <c r="FO7" s="27"/>
+      <c r="FP7" s="27"/>
+      <c r="FQ7" s="27"/>
+      <c r="FR7" s="27"/>
+      <c r="FS7" s="27"/>
+      <c r="FT7" s="27"/>
+      <c r="FU7" s="27"/>
+      <c r="FV7" s="27"/>
+      <c r="FW7" s="27"/>
+      <c r="FX7" s="27"/>
+      <c r="FY7" s="27"/>
+      <c r="FZ7" s="27"/>
+      <c r="GA7" s="27"/>
+      <c r="GB7" s="27"/>
+      <c r="GC7" s="27"/>
+      <c r="GD7" s="27"/>
+      <c r="GE7" s="27"/>
+      <c r="GF7" s="27"/>
+      <c r="GG7" s="27"/>
+      <c r="GH7" s="27"/>
+      <c r="GI7" s="27"/>
+      <c r="GJ7" s="27"/>
+      <c r="GK7" s="27"/>
+      <c r="GL7" s="27"/>
+      <c r="GM7" s="27"/>
+      <c r="GN7" s="27"/>
+      <c r="GO7" s="27"/>
+      <c r="GP7" s="27"/>
+      <c r="GQ7" s="27"/>
+      <c r="GR7" s="27"/>
+      <c r="GS7" s="27"/>
+      <c r="GT7" s="27"/>
+      <c r="GU7" s="27"/>
+      <c r="GV7" s="27"/>
+      <c r="GW7" s="27"/>
+      <c r="GX7" s="27"/>
+      <c r="GY7" s="27"/>
+      <c r="GZ7" s="27"/>
+      <c r="HA7" s="27"/>
+      <c r="HB7" s="27"/>
+      <c r="HC7" s="27"/>
+      <c r="HD7" s="27"/>
+      <c r="HE7" s="27"/>
+      <c r="HF7" s="27"/>
+      <c r="HG7" s="27"/>
+      <c r="HH7" s="27"/>
+      <c r="HI7" s="27"/>
+      <c r="HJ7" s="27"/>
+      <c r="HK7" s="27"/>
+      <c r="HL7" s="27"/>
+      <c r="HM7" s="27"/>
+      <c r="HN7" s="27"/>
+      <c r="HO7" s="27"/>
+      <c r="HP7" s="27"/>
+      <c r="HQ7" s="27"/>
+      <c r="HR7" s="27"/>
+      <c r="HS7" s="27"/>
+      <c r="HT7" s="27"/>
+      <c r="HU7" s="27"/>
+      <c r="HV7" s="27"/>
+      <c r="HW7" s="27"/>
+      <c r="HX7" s="27"/>
+      <c r="HY7" s="27"/>
+      <c r="HZ7" s="27"/>
+      <c r="IA7" s="27"/>
+      <c r="IB7" s="27"/>
+      <c r="IC7" s="27"/>
+      <c r="ID7" s="27"/>
+      <c r="IE7" s="27"/>
+      <c r="IF7" s="27"/>
+      <c r="IG7" s="27"/>
+      <c r="IH7" s="27"/>
+      <c r="II7" s="27"/>
+      <c r="IJ7" s="27"/>
+      <c r="IK7" s="27"/>
+      <c r="IL7" s="27"/>
+      <c r="IM7" s="27"/>
+      <c r="IN7" s="27"/>
+      <c r="IO7" s="27"/>
+      <c r="IP7" s="27"/>
+      <c r="IQ7" s="27"/>
+      <c r="IR7" s="27"/>
+      <c r="IS7" s="27"/>
+      <c r="IT7" s="27"/>
+      <c r="IU7" s="27"/>
+      <c r="IV7" s="27"/>
+      <c r="IW7" s="27"/>
+      <c r="IX7" s="27"/>
+      <c r="IY7" s="27"/>
+      <c r="IZ7" s="27"/>
+    </row>
+    <row r="8" spans="1:260" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="28" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
@@ -2889,275 +3291,39 @@
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
       <c r="L8" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="M8" s="27"/>
-      <c r="N8" s="27"/>
-      <c r="O8" s="27"/>
-      <c r="P8" s="27"/>
-      <c r="Q8" s="27"/>
-      <c r="R8" s="27"/>
-      <c r="S8" s="27"/>
-      <c r="T8" s="27"/>
-      <c r="U8" s="27"/>
-      <c r="V8" s="27"/>
-      <c r="W8" s="27"/>
-      <c r="X8" s="27"/>
-      <c r="Y8" s="27"/>
-      <c r="Z8" s="27"/>
-      <c r="AA8" s="27"/>
-      <c r="AB8" s="27"/>
-      <c r="AC8" s="27"/>
-      <c r="AD8" s="27"/>
-      <c r="AE8" s="27"/>
-      <c r="AF8" s="27"/>
-      <c r="AG8" s="27"/>
-      <c r="AH8" s="27"/>
-      <c r="AI8" s="27"/>
-      <c r="AJ8" s="27"/>
-      <c r="AK8" s="27"/>
-      <c r="AL8" s="27"/>
-      <c r="AM8" s="27"/>
-      <c r="AN8" s="27"/>
-      <c r="AO8" s="27"/>
-      <c r="AP8" s="27"/>
-      <c r="AQ8" s="27"/>
-      <c r="AR8" s="27"/>
-      <c r="AS8" s="27"/>
-      <c r="AT8" s="27"/>
-      <c r="AU8" s="27"/>
-      <c r="AV8" s="27"/>
-      <c r="AW8" s="27"/>
-      <c r="AX8" s="27"/>
-      <c r="AY8" s="27"/>
-      <c r="AZ8" s="27"/>
-      <c r="BA8" s="27"/>
-      <c r="BB8" s="27"/>
-      <c r="BC8" s="27"/>
-      <c r="BD8" s="27"/>
-      <c r="BE8" s="27"/>
-      <c r="BF8" s="27"/>
-      <c r="BG8" s="27"/>
-      <c r="BH8" s="27"/>
-      <c r="BI8" s="27"/>
-      <c r="BJ8" s="27"/>
-      <c r="BK8" s="27"/>
-      <c r="BL8" s="27"/>
-      <c r="BM8" s="27"/>
-      <c r="BN8" s="27"/>
-      <c r="BO8" s="27"/>
-      <c r="BP8" s="27"/>
-      <c r="BQ8" s="27"/>
-      <c r="BR8" s="27"/>
-      <c r="BS8" s="27"/>
-      <c r="BT8" s="27"/>
-      <c r="BU8" s="27"/>
-      <c r="BV8" s="27"/>
-      <c r="BW8" s="27"/>
-      <c r="BX8" s="27"/>
-      <c r="BY8" s="27"/>
-      <c r="BZ8" s="27"/>
-      <c r="CA8" s="27"/>
-      <c r="CB8" s="27"/>
-      <c r="CC8" s="27"/>
-      <c r="CD8" s="27"/>
-      <c r="CE8" s="27"/>
-      <c r="CF8" s="27"/>
-      <c r="CG8" s="27"/>
-      <c r="CH8" s="27"/>
-      <c r="CI8" s="27"/>
-      <c r="CJ8" s="27"/>
-      <c r="CK8" s="27"/>
-      <c r="CL8" s="27"/>
-      <c r="CM8" s="27"/>
-      <c r="CN8" s="27"/>
-      <c r="CO8" s="27"/>
-      <c r="CP8" s="27"/>
-      <c r="CQ8" s="27"/>
-      <c r="CR8" s="27"/>
-      <c r="CS8" s="27"/>
-      <c r="CT8" s="27"/>
-      <c r="CU8" s="27"/>
-      <c r="CV8" s="27"/>
-      <c r="CW8" s="27"/>
-      <c r="CX8" s="27"/>
-      <c r="CY8" s="27"/>
-      <c r="CZ8" s="27"/>
-      <c r="DA8" s="27"/>
-      <c r="DB8" s="27"/>
-      <c r="DC8" s="27"/>
-      <c r="DD8" s="27"/>
-      <c r="DE8" s="27"/>
-      <c r="DF8" s="27"/>
-      <c r="DG8" s="27"/>
-      <c r="DH8" s="27"/>
-      <c r="DI8" s="27"/>
-      <c r="DJ8" s="27"/>
-      <c r="DK8" s="27"/>
-      <c r="DL8" s="27"/>
-      <c r="DM8" s="27"/>
-      <c r="DN8" s="27"/>
-      <c r="DO8" s="27"/>
-      <c r="DP8" s="27"/>
-      <c r="DQ8" s="27"/>
-      <c r="DR8" s="27"/>
-      <c r="DS8" s="27"/>
-      <c r="DT8" s="27"/>
-      <c r="DU8" s="27"/>
-      <c r="DV8" s="27"/>
-      <c r="DW8" s="27"/>
-      <c r="DX8" s="27"/>
-      <c r="DY8" s="27"/>
-      <c r="DZ8" s="27"/>
-      <c r="EA8" s="27"/>
-      <c r="EB8" s="27"/>
-      <c r="EC8" s="27"/>
-      <c r="ED8" s="27"/>
-      <c r="EE8" s="27"/>
-      <c r="EF8" s="27"/>
-      <c r="EG8" s="27"/>
-      <c r="EH8" s="27"/>
-      <c r="EI8" s="27"/>
-      <c r="EJ8" s="27"/>
-      <c r="EK8" s="27"/>
-      <c r="EL8" s="27"/>
-      <c r="EM8" s="27"/>
-      <c r="EN8" s="27"/>
-      <c r="EO8" s="27"/>
-      <c r="EP8" s="27"/>
-      <c r="EQ8" s="27"/>
-      <c r="ER8" s="27"/>
-      <c r="ES8" s="27"/>
-      <c r="ET8" s="27"/>
-      <c r="EU8" s="27"/>
-      <c r="EV8" s="27"/>
-      <c r="EW8" s="27"/>
-      <c r="EX8" s="27"/>
-      <c r="EY8" s="27"/>
-      <c r="EZ8" s="27"/>
-      <c r="FA8" s="27"/>
-      <c r="FB8" s="27"/>
-      <c r="FC8" s="27"/>
-      <c r="FD8" s="27"/>
-      <c r="FE8" s="27"/>
-      <c r="FF8" s="27"/>
-      <c r="FG8" s="27"/>
-      <c r="FH8" s="27"/>
-      <c r="FI8" s="27"/>
-      <c r="FJ8" s="27"/>
-      <c r="FK8" s="27"/>
-      <c r="FL8" s="27"/>
-      <c r="FM8" s="27"/>
-      <c r="FN8" s="27"/>
-      <c r="FO8" s="27"/>
-      <c r="FP8" s="27"/>
-      <c r="FQ8" s="27"/>
-      <c r="FR8" s="27"/>
-      <c r="FS8" s="27"/>
-      <c r="FT8" s="27"/>
-      <c r="FU8" s="27"/>
-      <c r="FV8" s="27"/>
-      <c r="FW8" s="27"/>
-      <c r="FX8" s="27"/>
-      <c r="FY8" s="27"/>
-      <c r="FZ8" s="27"/>
-      <c r="GA8" s="27"/>
-      <c r="GB8" s="27"/>
-      <c r="GC8" s="27"/>
-      <c r="GD8" s="27"/>
-      <c r="GE8" s="27"/>
-      <c r="GF8" s="27"/>
-      <c r="GG8" s="27"/>
-      <c r="GH8" s="27"/>
-      <c r="GI8" s="27"/>
-      <c r="GJ8" s="27"/>
-      <c r="GK8" s="27"/>
-      <c r="GL8" s="27"/>
-      <c r="GM8" s="27"/>
-      <c r="GN8" s="27"/>
-      <c r="GO8" s="27"/>
-      <c r="GP8" s="27"/>
-      <c r="GQ8" s="27"/>
-      <c r="GR8" s="27"/>
-      <c r="GS8" s="27"/>
-      <c r="GT8" s="27"/>
-      <c r="GU8" s="27"/>
-      <c r="GV8" s="27"/>
-      <c r="GW8" s="27"/>
-      <c r="GX8" s="27"/>
-      <c r="GY8" s="27"/>
-      <c r="GZ8" s="27"/>
-      <c r="HA8" s="27"/>
-      <c r="HB8" s="27"/>
-      <c r="HC8" s="27"/>
-      <c r="HD8" s="27"/>
-      <c r="HE8" s="27"/>
-      <c r="HF8" s="27"/>
-      <c r="HG8" s="27"/>
-      <c r="HH8" s="27"/>
-      <c r="HI8" s="27"/>
-      <c r="HJ8" s="27"/>
-      <c r="HK8" s="27"/>
-      <c r="HL8" s="27"/>
-      <c r="HM8" s="27"/>
-      <c r="HN8" s="27"/>
-      <c r="HO8" s="27"/>
-      <c r="HP8" s="27"/>
-      <c r="HQ8" s="27"/>
-      <c r="HR8" s="27"/>
-      <c r="HS8" s="27"/>
-      <c r="HT8" s="27"/>
-      <c r="HU8" s="27"/>
-      <c r="HV8" s="27"/>
-      <c r="HW8" s="27"/>
-      <c r="HX8" s="27"/>
-      <c r="HY8" s="27"/>
-      <c r="HZ8" s="27"/>
-      <c r="IA8" s="27"/>
-      <c r="IB8" s="27"/>
-      <c r="IC8" s="27"/>
-      <c r="ID8" s="27"/>
-      <c r="IE8" s="27"/>
-      <c r="IF8" s="27"/>
-      <c r="IG8" s="27"/>
-      <c r="IH8" s="27"/>
-      <c r="II8" s="27"/>
-      <c r="IJ8" s="27"/>
-      <c r="IK8" s="27"/>
-      <c r="IL8" s="27"/>
-      <c r="IM8" s="27"/>
-      <c r="IN8" s="27"/>
-      <c r="IO8" s="27"/>
-      <c r="IP8" s="27"/>
-      <c r="IQ8" s="27"/>
-      <c r="IR8" s="27"/>
-      <c r="IS8" s="27"/>
-      <c r="IT8" s="27"/>
-      <c r="IU8" s="27"/>
-      <c r="IV8" s="27"/>
-      <c r="IW8" s="27"/>
-      <c r="IX8" s="27"/>
-      <c r="IY8" s="27"/>
-      <c r="IZ8" s="27"/>
+        <v>107</v>
+      </c>
     </row>
     <row r="9" spans="1:260" s="1" customFormat="1" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="29" t="s">
-        <v>104</v>
+      <c r="A9" s="28" t="s">
+        <v>99</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
+        <v>179</v>
+      </c>
+      <c r="C9" s="10">
+        <v>5</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>173</v>
+      </c>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
       <c r="L9" s="9" t="s">
-        <v>118</v>
+        <v>222</v>
       </c>
       <c r="M9" s="27"/>
       <c r="N9" s="27"/>
@@ -3409,11 +3575,11 @@
       <c r="IZ9" s="27"/>
     </row>
     <row r="10" spans="1:260" s="1" customFormat="1" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="28" t="s">
-        <v>105</v>
+      <c r="A10" s="29" t="s">
+        <v>100</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
@@ -3425,7 +3591,7 @@
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
       <c r="L10" s="9" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="M10" s="27"/>
       <c r="N10" s="27"/>
@@ -3678,10 +3844,10 @@
     </row>
     <row r="11" spans="1:260" s="1" customFormat="1" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="28" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
@@ -3693,7 +3859,7 @@
       <c r="J11" s="10"/>
       <c r="K11" s="10"/>
       <c r="L11" s="9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M11" s="27"/>
       <c r="N11" s="27"/>
@@ -3946,14 +4112,20 @@
     </row>
     <row r="12" spans="1:260" s="1" customFormat="1" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="28" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
+        <v>92</v>
+      </c>
+      <c r="C12" s="10">
+        <v>2</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>176</v>
+      </c>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
@@ -3961,7 +4133,7 @@
       <c r="J12" s="10"/>
       <c r="K12" s="10"/>
       <c r="L12" s="9" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="M12" s="27"/>
       <c r="N12" s="27"/>
@@ -4214,14 +4386,20 @@
     </row>
     <row r="13" spans="1:260" s="1" customFormat="1" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="28" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
+        <v>93</v>
+      </c>
+      <c r="C13" s="10">
+        <v>2</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>177</v>
+      </c>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
@@ -4229,7 +4407,7 @@
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
       <c r="L13" s="9" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="M13" s="27"/>
       <c r="N13" s="27"/>
@@ -4480,9 +4658,13 @@
       <c r="IY13" s="27"/>
       <c r="IZ13" s="27"/>
     </row>
-    <row r="14" spans="1:260" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="11"/>
-      <c r="B14" s="10"/>
+    <row r="14" spans="1:260" s="1" customFormat="1" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>94</v>
+      </c>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
@@ -4492,15 +4674,261 @@
       <c r="I14" s="10"/>
       <c r="J14" s="10"/>
       <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
+      <c r="L14" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="M14" s="27"/>
+      <c r="N14" s="27"/>
+      <c r="O14" s="27"/>
+      <c r="P14" s="27"/>
+      <c r="Q14" s="27"/>
+      <c r="R14" s="27"/>
+      <c r="S14" s="27"/>
+      <c r="T14" s="27"/>
+      <c r="U14" s="27"/>
+      <c r="V14" s="27"/>
+      <c r="W14" s="27"/>
+      <c r="X14" s="27"/>
+      <c r="Y14" s="27"/>
+      <c r="Z14" s="27"/>
+      <c r="AA14" s="27"/>
+      <c r="AB14" s="27"/>
+      <c r="AC14" s="27"/>
+      <c r="AD14" s="27"/>
+      <c r="AE14" s="27"/>
+      <c r="AF14" s="27"/>
+      <c r="AG14" s="27"/>
+      <c r="AH14" s="27"/>
+      <c r="AI14" s="27"/>
+      <c r="AJ14" s="27"/>
+      <c r="AK14" s="27"/>
+      <c r="AL14" s="27"/>
+      <c r="AM14" s="27"/>
+      <c r="AN14" s="27"/>
+      <c r="AO14" s="27"/>
+      <c r="AP14" s="27"/>
+      <c r="AQ14" s="27"/>
+      <c r="AR14" s="27"/>
+      <c r="AS14" s="27"/>
+      <c r="AT14" s="27"/>
+      <c r="AU14" s="27"/>
+      <c r="AV14" s="27"/>
+      <c r="AW14" s="27"/>
+      <c r="AX14" s="27"/>
+      <c r="AY14" s="27"/>
+      <c r="AZ14" s="27"/>
+      <c r="BA14" s="27"/>
+      <c r="BB14" s="27"/>
+      <c r="BC14" s="27"/>
+      <c r="BD14" s="27"/>
+      <c r="BE14" s="27"/>
+      <c r="BF14" s="27"/>
+      <c r="BG14" s="27"/>
+      <c r="BH14" s="27"/>
+      <c r="BI14" s="27"/>
+      <c r="BJ14" s="27"/>
+      <c r="BK14" s="27"/>
+      <c r="BL14" s="27"/>
+      <c r="BM14" s="27"/>
+      <c r="BN14" s="27"/>
+      <c r="BO14" s="27"/>
+      <c r="BP14" s="27"/>
+      <c r="BQ14" s="27"/>
+      <c r="BR14" s="27"/>
+      <c r="BS14" s="27"/>
+      <c r="BT14" s="27"/>
+      <c r="BU14" s="27"/>
+      <c r="BV14" s="27"/>
+      <c r="BW14" s="27"/>
+      <c r="BX14" s="27"/>
+      <c r="BY14" s="27"/>
+      <c r="BZ14" s="27"/>
+      <c r="CA14" s="27"/>
+      <c r="CB14" s="27"/>
+      <c r="CC14" s="27"/>
+      <c r="CD14" s="27"/>
+      <c r="CE14" s="27"/>
+      <c r="CF14" s="27"/>
+      <c r="CG14" s="27"/>
+      <c r="CH14" s="27"/>
+      <c r="CI14" s="27"/>
+      <c r="CJ14" s="27"/>
+      <c r="CK14" s="27"/>
+      <c r="CL14" s="27"/>
+      <c r="CM14" s="27"/>
+      <c r="CN14" s="27"/>
+      <c r="CO14" s="27"/>
+      <c r="CP14" s="27"/>
+      <c r="CQ14" s="27"/>
+      <c r="CR14" s="27"/>
+      <c r="CS14" s="27"/>
+      <c r="CT14" s="27"/>
+      <c r="CU14" s="27"/>
+      <c r="CV14" s="27"/>
+      <c r="CW14" s="27"/>
+      <c r="CX14" s="27"/>
+      <c r="CY14" s="27"/>
+      <c r="CZ14" s="27"/>
+      <c r="DA14" s="27"/>
+      <c r="DB14" s="27"/>
+      <c r="DC14" s="27"/>
+      <c r="DD14" s="27"/>
+      <c r="DE14" s="27"/>
+      <c r="DF14" s="27"/>
+      <c r="DG14" s="27"/>
+      <c r="DH14" s="27"/>
+      <c r="DI14" s="27"/>
+      <c r="DJ14" s="27"/>
+      <c r="DK14" s="27"/>
+      <c r="DL14" s="27"/>
+      <c r="DM14" s="27"/>
+      <c r="DN14" s="27"/>
+      <c r="DO14" s="27"/>
+      <c r="DP14" s="27"/>
+      <c r="DQ14" s="27"/>
+      <c r="DR14" s="27"/>
+      <c r="DS14" s="27"/>
+      <c r="DT14" s="27"/>
+      <c r="DU14" s="27"/>
+      <c r="DV14" s="27"/>
+      <c r="DW14" s="27"/>
+      <c r="DX14" s="27"/>
+      <c r="DY14" s="27"/>
+      <c r="DZ14" s="27"/>
+      <c r="EA14" s="27"/>
+      <c r="EB14" s="27"/>
+      <c r="EC14" s="27"/>
+      <c r="ED14" s="27"/>
+      <c r="EE14" s="27"/>
+      <c r="EF14" s="27"/>
+      <c r="EG14" s="27"/>
+      <c r="EH14" s="27"/>
+      <c r="EI14" s="27"/>
+      <c r="EJ14" s="27"/>
+      <c r="EK14" s="27"/>
+      <c r="EL14" s="27"/>
+      <c r="EM14" s="27"/>
+      <c r="EN14" s="27"/>
+      <c r="EO14" s="27"/>
+      <c r="EP14" s="27"/>
+      <c r="EQ14" s="27"/>
+      <c r="ER14" s="27"/>
+      <c r="ES14" s="27"/>
+      <c r="ET14" s="27"/>
+      <c r="EU14" s="27"/>
+      <c r="EV14" s="27"/>
+      <c r="EW14" s="27"/>
+      <c r="EX14" s="27"/>
+      <c r="EY14" s="27"/>
+      <c r="EZ14" s="27"/>
+      <c r="FA14" s="27"/>
+      <c r="FB14" s="27"/>
+      <c r="FC14" s="27"/>
+      <c r="FD14" s="27"/>
+      <c r="FE14" s="27"/>
+      <c r="FF14" s="27"/>
+      <c r="FG14" s="27"/>
+      <c r="FH14" s="27"/>
+      <c r="FI14" s="27"/>
+      <c r="FJ14" s="27"/>
+      <c r="FK14" s="27"/>
+      <c r="FL14" s="27"/>
+      <c r="FM14" s="27"/>
+      <c r="FN14" s="27"/>
+      <c r="FO14" s="27"/>
+      <c r="FP14" s="27"/>
+      <c r="FQ14" s="27"/>
+      <c r="FR14" s="27"/>
+      <c r="FS14" s="27"/>
+      <c r="FT14" s="27"/>
+      <c r="FU14" s="27"/>
+      <c r="FV14" s="27"/>
+      <c r="FW14" s="27"/>
+      <c r="FX14" s="27"/>
+      <c r="FY14" s="27"/>
+      <c r="FZ14" s="27"/>
+      <c r="GA14" s="27"/>
+      <c r="GB14" s="27"/>
+      <c r="GC14" s="27"/>
+      <c r="GD14" s="27"/>
+      <c r="GE14" s="27"/>
+      <c r="GF14" s="27"/>
+      <c r="GG14" s="27"/>
+      <c r="GH14" s="27"/>
+      <c r="GI14" s="27"/>
+      <c r="GJ14" s="27"/>
+      <c r="GK14" s="27"/>
+      <c r="GL14" s="27"/>
+      <c r="GM14" s="27"/>
+      <c r="GN14" s="27"/>
+      <c r="GO14" s="27"/>
+      <c r="GP14" s="27"/>
+      <c r="GQ14" s="27"/>
+      <c r="GR14" s="27"/>
+      <c r="GS14" s="27"/>
+      <c r="GT14" s="27"/>
+      <c r="GU14" s="27"/>
+      <c r="GV14" s="27"/>
+      <c r="GW14" s="27"/>
+      <c r="GX14" s="27"/>
+      <c r="GY14" s="27"/>
+      <c r="GZ14" s="27"/>
+      <c r="HA14" s="27"/>
+      <c r="HB14" s="27"/>
+      <c r="HC14" s="27"/>
+      <c r="HD14" s="27"/>
+      <c r="HE14" s="27"/>
+      <c r="HF14" s="27"/>
+      <c r="HG14" s="27"/>
+      <c r="HH14" s="27"/>
+      <c r="HI14" s="27"/>
+      <c r="HJ14" s="27"/>
+      <c r="HK14" s="27"/>
+      <c r="HL14" s="27"/>
+      <c r="HM14" s="27"/>
+      <c r="HN14" s="27"/>
+      <c r="HO14" s="27"/>
+      <c r="HP14" s="27"/>
+      <c r="HQ14" s="27"/>
+      <c r="HR14" s="27"/>
+      <c r="HS14" s="27"/>
+      <c r="HT14" s="27"/>
+      <c r="HU14" s="27"/>
+      <c r="HV14" s="27"/>
+      <c r="HW14" s="27"/>
+      <c r="HX14" s="27"/>
+      <c r="HY14" s="27"/>
+      <c r="HZ14" s="27"/>
+      <c r="IA14" s="27"/>
+      <c r="IB14" s="27"/>
+      <c r="IC14" s="27"/>
+      <c r="ID14" s="27"/>
+      <c r="IE14" s="27"/>
+      <c r="IF14" s="27"/>
+      <c r="IG14" s="27"/>
+      <c r="IH14" s="27"/>
+      <c r="II14" s="27"/>
+      <c r="IJ14" s="27"/>
+      <c r="IK14" s="27"/>
+      <c r="IL14" s="27"/>
+      <c r="IM14" s="27"/>
+      <c r="IN14" s="27"/>
+      <c r="IO14" s="27"/>
+      <c r="IP14" s="27"/>
+      <c r="IQ14" s="27"/>
+      <c r="IR14" s="27"/>
+      <c r="IS14" s="27"/>
+      <c r="IT14" s="27"/>
+      <c r="IU14" s="27"/>
+      <c r="IV14" s="27"/>
+      <c r="IW14" s="27"/>
+      <c r="IX14" s="27"/>
+      <c r="IY14" s="27"/>
+      <c r="IZ14" s="27"/>
     </row>
     <row r="15" spans="1:260" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>16</v>
-      </c>
+      <c r="A15" s="11"/>
+      <c r="B15" s="10"/>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
@@ -4514,10 +4942,10 @@
     </row>
     <row r="16" spans="1:260" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
@@ -4531,11 +4959,11 @@
       <c r="L16" s="10"/>
     </row>
     <row r="17" spans="1:12" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="13" t="s">
-        <v>19</v>
+      <c r="A17" s="12" t="s">
+        <v>17</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
@@ -4550,10 +4978,10 @@
     </row>
     <row r="18" spans="1:12" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
@@ -4567,8 +4995,12 @@
       <c r="L18" s="10"/>
     </row>
     <row r="19" spans="1:12" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="11"/>
-      <c r="B19" s="10"/>
+      <c r="A19" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>22</v>
+      </c>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
@@ -4581,7 +5013,7 @@
       <c r="L19" s="10"/>
     </row>
     <row r="20" spans="1:12" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="14"/>
+      <c r="A20" s="11"/>
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
@@ -4623,18 +5055,10 @@
       <c r="L22" s="10"/>
     </row>
     <row r="23" spans="1:12" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" s="9">
-        <v>1</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>25</v>
-      </c>
+      <c r="A23" s="14"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
@@ -4642,80 +5066,82 @@
       <c r="I23" s="10"/>
       <c r="J23" s="10"/>
       <c r="K23" s="10"/>
-      <c r="L23" s="16" t="s">
-        <v>26</v>
-      </c>
+      <c r="L23" s="10"/>
     </row>
     <row r="24" spans="1:12" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C24" s="9">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F24" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="9" t="s">
-        <v>33</v>
+        <v>25</v>
+      </c>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="16" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C25" s="9">
+        <v>6</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="9">
+        <v>2</v>
+      </c>
+      <c r="D26" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="E26" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C25" s="9">
-        <v>2</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="10"/>
-      <c r="L25" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="C26" s="9">
-        <v>1</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="E26" s="10"/>
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
       <c r="H26" s="10"/>
@@ -4723,21 +5149,21 @@
       <c r="J26" s="10"/>
       <c r="K26" s="10"/>
       <c r="L26" s="9" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="15" t="s">
-        <v>43</v>
+      <c r="A27" s="17" t="s">
+        <v>37</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>44</v>
+        <v>186</v>
       </c>
       <c r="C27" s="9">
         <v>1</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
@@ -4747,14 +5173,22 @@
       <c r="J27" s="10"/>
       <c r="K27" s="10"/>
       <c r="L27" s="9" t="s">
-        <v>46</v>
+        <v>192</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="11"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
+      <c r="A28" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="C28" s="9">
+        <v>1</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>42</v>
+      </c>
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
@@ -4762,13 +5196,23 @@
       <c r="I28" s="10"/>
       <c r="J28" s="10"/>
       <c r="K28" s="10"/>
-      <c r="L28" s="10"/>
+      <c r="L28" s="9" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="29" spans="1:12" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="11"/>
-      <c r="B29" s="9"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
+      <c r="A29" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="C29" s="9">
+        <v>1</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>39</v>
+      </c>
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
@@ -4776,13 +5220,23 @@
       <c r="I29" s="10"/>
       <c r="J29" s="10"/>
       <c r="K29" s="10"/>
-      <c r="L29" s="9"/>
+      <c r="L29" s="9" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="30" spans="1:12" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="11"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
+      <c r="A30" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="C30" s="9">
+        <v>1</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>42</v>
+      </c>
       <c r="E30" s="10"/>
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
@@ -4790,13 +5244,23 @@
       <c r="I30" s="10"/>
       <c r="J30" s="10"/>
       <c r="K30" s="10"/>
-      <c r="L30" s="9"/>
+      <c r="L30" s="9" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="31" spans="1:12" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="11"/>
-      <c r="B31" s="9"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
+      <c r="A31" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="C31" s="9">
+        <v>1</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>39</v>
+      </c>
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
       <c r="G31" s="10"/>
@@ -4804,20 +5268,22 @@
       <c r="I31" s="10"/>
       <c r="J31" s="10"/>
       <c r="K31" s="10"/>
-      <c r="L31" s="9"/>
+      <c r="L31" s="9" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="32" spans="1:12" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="18" t="s">
-        <v>47</v>
+      <c r="A32" s="15" t="s">
+        <v>198</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>48</v>
+        <v>196</v>
       </c>
       <c r="C32" s="9">
         <v>1</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="E32" s="10"/>
       <c r="F32" s="10"/>
@@ -4827,21 +5293,21 @@
       <c r="J32" s="10"/>
       <c r="K32" s="10"/>
       <c r="L32" s="9" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:260" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="18" t="s">
-        <v>51</v>
+      <c r="A33" s="17" t="s">
+        <v>199</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>52</v>
+        <v>204</v>
       </c>
       <c r="C33" s="9">
         <v>1</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="E33" s="10"/>
       <c r="F33" s="10"/>
@@ -4851,42 +5317,46 @@
       <c r="J33" s="10"/>
       <c r="K33" s="10"/>
       <c r="L33" s="9" t="s">
-        <v>53</v>
+        <v>209</v>
       </c>
     </row>
     <row r="34" spans="1:260" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="18" t="s">
-        <v>54</v>
+      <c r="A34" s="15" t="s">
+        <v>200</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>55</v>
+        <v>197</v>
       </c>
       <c r="C34" s="9">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="E34" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="F34" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="G34" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="H34" s="9"/>
-      <c r="I34" s="9"/>
-      <c r="J34" s="9"/>
-      <c r="K34" s="9"/>
-      <c r="L34" s="9"/>
+        <v>42</v>
+      </c>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="10"/>
+      <c r="L34" s="9" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="35" spans="1:260" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="11"/>
-      <c r="B35" s="9"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
+      <c r="A35" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="C35" s="9">
+        <v>1</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>39</v>
+      </c>
       <c r="E35" s="10"/>
       <c r="F35" s="10"/>
       <c r="G35" s="10"/>
@@ -4894,785 +5364,1291 @@
       <c r="I35" s="10"/>
       <c r="J35" s="10"/>
       <c r="K35" s="10"/>
-      <c r="L35" s="33"/>
+      <c r="L35" s="9" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="36" spans="1:260" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="40" t="s">
-        <v>156</v>
-      </c>
-      <c r="B36" s="9"/>
-      <c r="C36" s="10">
-        <v>8</v>
-      </c>
-      <c r="D36" s="10"/>
+      <c r="A36" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C36" s="9">
+        <v>1</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>42</v>
+      </c>
       <c r="E36" s="10"/>
       <c r="F36" s="10"/>
       <c r="G36" s="10"/>
       <c r="H36" s="10"/>
       <c r="I36" s="10"/>
       <c r="J36" s="10"/>
-      <c r="K36" s="37"/>
-      <c r="L36" s="39" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="37" spans="1:260" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="40" t="s">
-        <v>157</v>
-      </c>
-      <c r="B37" s="9"/>
-      <c r="C37" s="10">
-        <v>8</v>
-      </c>
-      <c r="D37" s="10"/>
+      <c r="K36" s="10"/>
+      <c r="L36" s="9" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="37" spans="1:260" s="30" customFormat="1" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="17" t="s">
+        <v>203</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="C37" s="9">
+        <v>1</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>39</v>
+      </c>
       <c r="E37" s="10"/>
       <c r="F37" s="10"/>
       <c r="G37" s="10"/>
       <c r="H37" s="10"/>
       <c r="I37" s="10"/>
       <c r="J37" s="10"/>
-      <c r="K37" s="37"/>
-      <c r="L37" s="39"/>
+      <c r="K37" s="10"/>
+      <c r="L37" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="M37" s="27"/>
+      <c r="N37" s="27"/>
+      <c r="O37" s="27"/>
+      <c r="P37" s="27"/>
+      <c r="Q37" s="27"/>
+      <c r="R37" s="27"/>
+      <c r="S37" s="27"/>
+      <c r="T37" s="27"/>
+      <c r="U37" s="27"/>
+      <c r="V37" s="27"/>
+      <c r="W37" s="27"/>
+      <c r="X37" s="27"/>
+      <c r="Y37" s="27"/>
+      <c r="Z37" s="27"/>
+      <c r="AA37" s="27"/>
+      <c r="AB37" s="27"/>
+      <c r="AC37" s="27"/>
+      <c r="AD37" s="27"/>
+      <c r="AE37" s="27"/>
+      <c r="AF37" s="27"/>
+      <c r="AG37" s="27"/>
+      <c r="AH37" s="27"/>
+      <c r="AI37" s="27"/>
+      <c r="AJ37" s="27"/>
+      <c r="AK37" s="27"/>
+      <c r="AL37" s="27"/>
+      <c r="AM37" s="27"/>
+      <c r="AN37" s="27"/>
+      <c r="AO37" s="27"/>
+      <c r="AP37" s="27"/>
+      <c r="AQ37" s="27"/>
+      <c r="AR37" s="27"/>
+      <c r="AS37" s="27"/>
+      <c r="AT37" s="27"/>
+      <c r="AU37" s="27"/>
+      <c r="AV37" s="27"/>
+      <c r="AW37" s="27"/>
+      <c r="AX37" s="27"/>
+      <c r="AY37" s="27"/>
+      <c r="AZ37" s="27"/>
+      <c r="BA37" s="27"/>
+      <c r="BB37" s="27"/>
+      <c r="BC37" s="27"/>
+      <c r="BD37" s="27"/>
+      <c r="BE37" s="27"/>
+      <c r="BF37" s="27"/>
+      <c r="BG37" s="27"/>
+      <c r="BH37" s="27"/>
+      <c r="BI37" s="27"/>
+      <c r="BJ37" s="27"/>
+      <c r="BK37" s="27"/>
+      <c r="BL37" s="27"/>
+      <c r="BM37" s="27"/>
+      <c r="BN37" s="27"/>
+      <c r="BO37" s="27"/>
+      <c r="BP37" s="27"/>
+      <c r="BQ37" s="27"/>
+      <c r="BR37" s="27"/>
+      <c r="BS37" s="27"/>
+      <c r="BT37" s="27"/>
+      <c r="BU37" s="27"/>
+      <c r="BV37" s="27"/>
+      <c r="BW37" s="27"/>
+      <c r="BX37" s="27"/>
+      <c r="BY37" s="27"/>
+      <c r="BZ37" s="27"/>
+      <c r="CA37" s="27"/>
+      <c r="CB37" s="27"/>
+      <c r="CC37" s="27"/>
+      <c r="CD37" s="27"/>
+      <c r="CE37" s="27"/>
+      <c r="CF37" s="27"/>
+      <c r="CG37" s="27"/>
+      <c r="CH37" s="27"/>
+      <c r="CI37" s="27"/>
+      <c r="CJ37" s="27"/>
+      <c r="CK37" s="27"/>
+      <c r="CL37" s="27"/>
+      <c r="CM37" s="27"/>
+      <c r="CN37" s="27"/>
+      <c r="CO37" s="27"/>
+      <c r="CP37" s="27"/>
+      <c r="CQ37" s="27"/>
+      <c r="CR37" s="27"/>
+      <c r="CS37" s="27"/>
+      <c r="CT37" s="27"/>
+      <c r="CU37" s="27"/>
+      <c r="CV37" s="27"/>
+      <c r="CW37" s="27"/>
+      <c r="CX37" s="27"/>
+      <c r="CY37" s="27"/>
+      <c r="CZ37" s="27"/>
+      <c r="DA37" s="27"/>
+      <c r="DB37" s="27"/>
+      <c r="DC37" s="27"/>
+      <c r="DD37" s="27"/>
+      <c r="DE37" s="27"/>
+      <c r="DF37" s="27"/>
+      <c r="DG37" s="27"/>
+      <c r="DH37" s="27"/>
+      <c r="DI37" s="27"/>
+      <c r="DJ37" s="27"/>
+      <c r="DK37" s="27"/>
+      <c r="DL37" s="27"/>
+      <c r="DM37" s="27"/>
+      <c r="DN37" s="27"/>
+      <c r="DO37" s="27"/>
+      <c r="DP37" s="27"/>
+      <c r="DQ37" s="27"/>
+      <c r="DR37" s="27"/>
+      <c r="DS37" s="27"/>
+      <c r="DT37" s="27"/>
+      <c r="DU37" s="27"/>
+      <c r="DV37" s="27"/>
+      <c r="DW37" s="27"/>
+      <c r="DX37" s="27"/>
+      <c r="DY37" s="27"/>
+      <c r="DZ37" s="27"/>
+      <c r="EA37" s="27"/>
+      <c r="EB37" s="27"/>
+      <c r="EC37" s="27"/>
+      <c r="ED37" s="27"/>
+      <c r="EE37" s="27"/>
+      <c r="EF37" s="27"/>
+      <c r="EG37" s="27"/>
+      <c r="EH37" s="27"/>
+      <c r="EI37" s="27"/>
+      <c r="EJ37" s="27"/>
+      <c r="EK37" s="27"/>
+      <c r="EL37" s="27"/>
+      <c r="EM37" s="27"/>
+      <c r="EN37" s="27"/>
+      <c r="EO37" s="27"/>
+      <c r="EP37" s="27"/>
+      <c r="EQ37" s="27"/>
+      <c r="ER37" s="27"/>
+      <c r="ES37" s="27"/>
+      <c r="ET37" s="27"/>
+      <c r="EU37" s="27"/>
+      <c r="EV37" s="27"/>
+      <c r="EW37" s="27"/>
+      <c r="EX37" s="27"/>
+      <c r="EY37" s="27"/>
+      <c r="EZ37" s="27"/>
+      <c r="FA37" s="27"/>
+      <c r="FB37" s="27"/>
+      <c r="FC37" s="27"/>
+      <c r="FD37" s="27"/>
+      <c r="FE37" s="27"/>
+      <c r="FF37" s="27"/>
+      <c r="FG37" s="27"/>
+      <c r="FH37" s="27"/>
+      <c r="FI37" s="27"/>
+      <c r="FJ37" s="27"/>
+      <c r="FK37" s="27"/>
+      <c r="FL37" s="27"/>
+      <c r="FM37" s="27"/>
+      <c r="FN37" s="27"/>
+      <c r="FO37" s="27"/>
+      <c r="FP37" s="27"/>
+      <c r="FQ37" s="27"/>
+      <c r="FR37" s="27"/>
+      <c r="FS37" s="27"/>
+      <c r="FT37" s="27"/>
+      <c r="FU37" s="27"/>
+      <c r="FV37" s="27"/>
+      <c r="FW37" s="27"/>
+      <c r="FX37" s="27"/>
+      <c r="FY37" s="27"/>
+      <c r="FZ37" s="27"/>
+      <c r="GA37" s="27"/>
+      <c r="GB37" s="27"/>
+      <c r="GC37" s="27"/>
+      <c r="GD37" s="27"/>
+      <c r="GE37" s="27"/>
+      <c r="GF37" s="27"/>
+      <c r="GG37" s="27"/>
+      <c r="GH37" s="27"/>
+      <c r="GI37" s="27"/>
+      <c r="GJ37" s="27"/>
+      <c r="GK37" s="27"/>
+      <c r="GL37" s="27"/>
+      <c r="GM37" s="27"/>
+      <c r="GN37" s="27"/>
+      <c r="GO37" s="27"/>
+      <c r="GP37" s="27"/>
+      <c r="GQ37" s="27"/>
+      <c r="GR37" s="27"/>
+      <c r="GS37" s="27"/>
+      <c r="GT37" s="27"/>
+      <c r="GU37" s="27"/>
+      <c r="GV37" s="27"/>
+      <c r="GW37" s="27"/>
+      <c r="GX37" s="27"/>
+      <c r="GY37" s="27"/>
+      <c r="GZ37" s="27"/>
+      <c r="HA37" s="27"/>
+      <c r="HB37" s="27"/>
+      <c r="HC37" s="27"/>
+      <c r="HD37" s="27"/>
+      <c r="HE37" s="27"/>
+      <c r="HF37" s="27"/>
+      <c r="HG37" s="27"/>
+      <c r="HH37" s="27"/>
+      <c r="HI37" s="27"/>
+      <c r="HJ37" s="27"/>
+      <c r="HK37" s="27"/>
+      <c r="HL37" s="27"/>
+      <c r="HM37" s="27"/>
+      <c r="HN37" s="27"/>
+      <c r="HO37" s="27"/>
+      <c r="HP37" s="27"/>
+      <c r="HQ37" s="27"/>
+      <c r="HR37" s="27"/>
+      <c r="HS37" s="27"/>
+      <c r="HT37" s="27"/>
+      <c r="HU37" s="27"/>
+      <c r="HV37" s="27"/>
+      <c r="HW37" s="27"/>
+      <c r="HX37" s="27"/>
+      <c r="HY37" s="27"/>
+      <c r="HZ37" s="27"/>
+      <c r="IA37" s="27"/>
+      <c r="IB37" s="27"/>
+      <c r="IC37" s="27"/>
+      <c r="ID37" s="27"/>
+      <c r="IE37" s="27"/>
+      <c r="IF37" s="27"/>
+      <c r="IG37" s="27"/>
+      <c r="IH37" s="27"/>
+      <c r="II37" s="27"/>
+      <c r="IJ37" s="27"/>
+      <c r="IK37" s="27"/>
+      <c r="IL37" s="27"/>
+      <c r="IM37" s="27"/>
+      <c r="IN37" s="27"/>
+      <c r="IO37" s="27"/>
+      <c r="IP37" s="27"/>
+      <c r="IQ37" s="27"/>
+      <c r="IR37" s="27"/>
+      <c r="IS37" s="27"/>
+      <c r="IT37" s="27"/>
+      <c r="IU37" s="27"/>
+      <c r="IV37" s="27"/>
+      <c r="IW37" s="27"/>
+      <c r="IX37" s="27"/>
+      <c r="IY37" s="27"/>
+      <c r="IZ37" s="27"/>
     </row>
     <row r="38" spans="1:260" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="40" t="s">
-        <v>158</v>
-      </c>
-      <c r="B38" s="9"/>
-      <c r="C38" s="10">
-        <v>6</v>
-      </c>
-      <c r="D38" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="E38" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="F38" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="G38" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="H38" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="I38" s="10" t="s">
-        <v>126</v>
-      </c>
+      <c r="A38" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="C38" s="9">
+        <v>1</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
+      <c r="H38" s="10"/>
+      <c r="I38" s="10"/>
       <c r="J38" s="10"/>
       <c r="K38" s="10"/>
-      <c r="L38" s="38"/>
+      <c r="L38" s="9" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="39" spans="1:260" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="40" t="s">
-        <v>159</v>
-      </c>
-      <c r="B39" s="9"/>
+      <c r="A39" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>218</v>
+      </c>
       <c r="C39" s="10">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="E39" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="F39" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="G39" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="H39" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="I39" s="10" t="s">
-        <v>132</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="10"/>
       <c r="J39" s="10"/>
       <c r="K39" s="10"/>
-      <c r="L39" s="9"/>
+      <c r="L39" s="10" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="40" spans="1:260" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="40" t="s">
-        <v>160</v>
-      </c>
+      <c r="A40" s="11"/>
       <c r="B40" s="9"/>
-      <c r="C40" s="10">
-        <v>6</v>
-      </c>
-      <c r="D40" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="E40" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="F40" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="G40" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="H40" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="I40" s="10" t="s">
-        <v>138</v>
-      </c>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="10"/>
       <c r="J40" s="10"/>
       <c r="K40" s="10"/>
       <c r="L40" s="9"/>
     </row>
     <row r="41" spans="1:260" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="40" t="s">
+      <c r="A41" s="11"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
+      <c r="I41" s="10"/>
+      <c r="J41" s="10"/>
+      <c r="K41" s="10"/>
+      <c r="L41" s="9"/>
+    </row>
+    <row r="42" spans="1:260" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="11"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10"/>
+      <c r="I42" s="10"/>
+      <c r="J42" s="10"/>
+      <c r="K42" s="10"/>
+      <c r="L42" s="9"/>
+    </row>
+    <row r="43" spans="1:260" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C43" s="9">
+        <v>1</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
+      <c r="H43" s="10"/>
+      <c r="I43" s="10"/>
+      <c r="J43" s="10"/>
+      <c r="K43" s="10"/>
+      <c r="L43" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44" spans="1:260" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C44" s="9">
+        <v>1</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E44" s="10"/>
+      <c r="F44" s="10"/>
+      <c r="G44" s="10"/>
+      <c r="H44" s="10"/>
+      <c r="I44" s="10"/>
+      <c r="J44" s="10"/>
+      <c r="K44" s="10"/>
+      <c r="L44" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="45" spans="1:260" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C45" s="9">
+        <v>4</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="G45" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="H45" s="9"/>
+      <c r="I45" s="9"/>
+      <c r="J45" s="9"/>
+      <c r="K45" s="9"/>
+      <c r="L45" s="9"/>
+    </row>
+    <row r="46" spans="1:260" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="C46" s="9">
+        <v>4</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E46" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F46" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="G46" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="H46" s="10"/>
+      <c r="I46" s="10"/>
+      <c r="J46" s="10"/>
+      <c r="K46" s="10"/>
+      <c r="L46" s="32"/>
+    </row>
+    <row r="47" spans="1:260" s="45" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="18"/>
+      <c r="B47" s="9"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
+      <c r="G47" s="9"/>
+      <c r="H47" s="10"/>
+      <c r="I47" s="10"/>
+      <c r="J47" s="10"/>
+      <c r="K47" s="36"/>
+      <c r="L47" s="48"/>
+      <c r="M47" s="44"/>
+      <c r="N47" s="44"/>
+      <c r="O47" s="44"/>
+      <c r="P47" s="44"/>
+      <c r="Q47" s="44"/>
+      <c r="R47" s="44"/>
+      <c r="S47" s="44"/>
+      <c r="T47" s="44"/>
+      <c r="U47" s="44"/>
+      <c r="V47" s="44"/>
+      <c r="W47" s="44"/>
+      <c r="X47" s="44"/>
+      <c r="Y47" s="44"/>
+      <c r="Z47" s="44"/>
+      <c r="AA47" s="44"/>
+      <c r="AB47" s="44"/>
+      <c r="AC47" s="44"/>
+      <c r="AD47" s="44"/>
+      <c r="AE47" s="44"/>
+      <c r="AF47" s="44"/>
+      <c r="AG47" s="44"/>
+      <c r="AH47" s="44"/>
+      <c r="AI47" s="44"/>
+      <c r="AJ47" s="44"/>
+      <c r="AK47" s="44"/>
+      <c r="AL47" s="44"/>
+      <c r="AM47" s="44"/>
+      <c r="AN47" s="44"/>
+      <c r="AO47" s="44"/>
+      <c r="AP47" s="44"/>
+      <c r="AQ47" s="44"/>
+      <c r="AR47" s="44"/>
+      <c r="AS47" s="44"/>
+      <c r="AT47" s="44"/>
+      <c r="AU47" s="44"/>
+      <c r="AV47" s="44"/>
+      <c r="AW47" s="44"/>
+      <c r="AX47" s="44"/>
+      <c r="AY47" s="44"/>
+      <c r="AZ47" s="44"/>
+      <c r="BA47" s="44"/>
+      <c r="BB47" s="44"/>
+      <c r="BC47" s="44"/>
+      <c r="BD47" s="44"/>
+      <c r="BE47" s="44"/>
+      <c r="BF47" s="44"/>
+      <c r="BG47" s="44"/>
+      <c r="BH47" s="44"/>
+      <c r="BI47" s="44"/>
+      <c r="BJ47" s="44"/>
+      <c r="BK47" s="44"/>
+      <c r="BL47" s="44"/>
+      <c r="BM47" s="44"/>
+      <c r="BN47" s="44"/>
+      <c r="BO47" s="44"/>
+      <c r="BP47" s="44"/>
+      <c r="BQ47" s="44"/>
+      <c r="BR47" s="44"/>
+      <c r="BS47" s="44"/>
+      <c r="BT47" s="44"/>
+      <c r="BU47" s="44"/>
+      <c r="BV47" s="44"/>
+      <c r="BW47" s="44"/>
+      <c r="BX47" s="44"/>
+      <c r="BY47" s="44"/>
+      <c r="BZ47" s="44"/>
+      <c r="CA47" s="44"/>
+      <c r="CB47" s="44"/>
+      <c r="CC47" s="44"/>
+      <c r="CD47" s="44"/>
+      <c r="CE47" s="44"/>
+      <c r="CF47" s="44"/>
+      <c r="CG47" s="44"/>
+      <c r="CH47" s="44"/>
+      <c r="CI47" s="44"/>
+      <c r="CJ47" s="44"/>
+      <c r="CK47" s="44"/>
+      <c r="CL47" s="44"/>
+      <c r="CM47" s="44"/>
+      <c r="CN47" s="44"/>
+      <c r="CO47" s="44"/>
+      <c r="CP47" s="44"/>
+      <c r="CQ47" s="44"/>
+      <c r="CR47" s="44"/>
+      <c r="CS47" s="44"/>
+      <c r="CT47" s="44"/>
+      <c r="CU47" s="44"/>
+      <c r="CV47" s="44"/>
+      <c r="CW47" s="44"/>
+      <c r="CX47" s="44"/>
+      <c r="CY47" s="44"/>
+      <c r="CZ47" s="44"/>
+      <c r="DA47" s="44"/>
+      <c r="DB47" s="44"/>
+      <c r="DC47" s="44"/>
+      <c r="DD47" s="44"/>
+      <c r="DE47" s="44"/>
+      <c r="DF47" s="44"/>
+      <c r="DG47" s="44"/>
+      <c r="DH47" s="44"/>
+      <c r="DI47" s="44"/>
+      <c r="DJ47" s="44"/>
+      <c r="DK47" s="44"/>
+      <c r="DL47" s="44"/>
+      <c r="DM47" s="44"/>
+      <c r="DN47" s="44"/>
+      <c r="DO47" s="44"/>
+      <c r="DP47" s="44"/>
+      <c r="DQ47" s="44"/>
+      <c r="DR47" s="44"/>
+      <c r="DS47" s="44"/>
+      <c r="DT47" s="44"/>
+      <c r="DU47" s="44"/>
+      <c r="DV47" s="44"/>
+      <c r="DW47" s="44"/>
+      <c r="DX47" s="44"/>
+      <c r="DY47" s="44"/>
+      <c r="DZ47" s="44"/>
+      <c r="EA47" s="44"/>
+      <c r="EB47" s="44"/>
+      <c r="EC47" s="44"/>
+      <c r="ED47" s="44"/>
+      <c r="EE47" s="44"/>
+      <c r="EF47" s="44"/>
+      <c r="EG47" s="44"/>
+      <c r="EH47" s="44"/>
+      <c r="EI47" s="44"/>
+      <c r="EJ47" s="44"/>
+      <c r="EK47" s="44"/>
+      <c r="EL47" s="44"/>
+      <c r="EM47" s="44"/>
+      <c r="EN47" s="44"/>
+      <c r="EO47" s="44"/>
+      <c r="EP47" s="44"/>
+      <c r="EQ47" s="44"/>
+      <c r="ER47" s="44"/>
+      <c r="ES47" s="44"/>
+      <c r="ET47" s="44"/>
+      <c r="EU47" s="44"/>
+      <c r="EV47" s="44"/>
+      <c r="EW47" s="44"/>
+      <c r="EX47" s="44"/>
+      <c r="EY47" s="44"/>
+      <c r="EZ47" s="44"/>
+      <c r="FA47" s="44"/>
+      <c r="FB47" s="44"/>
+      <c r="FC47" s="44"/>
+      <c r="FD47" s="44"/>
+      <c r="FE47" s="44"/>
+      <c r="FF47" s="44"/>
+      <c r="FG47" s="44"/>
+      <c r="FH47" s="44"/>
+      <c r="FI47" s="44"/>
+      <c r="FJ47" s="44"/>
+      <c r="FK47" s="44"/>
+      <c r="FL47" s="44"/>
+      <c r="FM47" s="44"/>
+      <c r="FN47" s="44"/>
+      <c r="FO47" s="44"/>
+      <c r="FP47" s="44"/>
+      <c r="FQ47" s="44"/>
+      <c r="FR47" s="44"/>
+      <c r="FS47" s="44"/>
+      <c r="FT47" s="44"/>
+      <c r="FU47" s="44"/>
+      <c r="FV47" s="44"/>
+      <c r="FW47" s="44"/>
+      <c r="FX47" s="44"/>
+      <c r="FY47" s="44"/>
+      <c r="FZ47" s="44"/>
+      <c r="GA47" s="44"/>
+      <c r="GB47" s="44"/>
+      <c r="GC47" s="44"/>
+      <c r="GD47" s="44"/>
+      <c r="GE47" s="44"/>
+      <c r="GF47" s="44"/>
+      <c r="GG47" s="44"/>
+      <c r="GH47" s="44"/>
+      <c r="GI47" s="44"/>
+      <c r="GJ47" s="44"/>
+      <c r="GK47" s="44"/>
+      <c r="GL47" s="44"/>
+      <c r="GM47" s="44"/>
+      <c r="GN47" s="44"/>
+      <c r="GO47" s="44"/>
+      <c r="GP47" s="44"/>
+      <c r="GQ47" s="44"/>
+      <c r="GR47" s="44"/>
+      <c r="GS47" s="44"/>
+      <c r="GT47" s="44"/>
+      <c r="GU47" s="44"/>
+      <c r="GV47" s="44"/>
+      <c r="GW47" s="44"/>
+      <c r="GX47" s="44"/>
+      <c r="GY47" s="44"/>
+      <c r="GZ47" s="44"/>
+      <c r="HA47" s="44"/>
+      <c r="HB47" s="44"/>
+      <c r="HC47" s="44"/>
+      <c r="HD47" s="44"/>
+      <c r="HE47" s="44"/>
+      <c r="HF47" s="44"/>
+      <c r="HG47" s="44"/>
+      <c r="HH47" s="44"/>
+      <c r="HI47" s="44"/>
+      <c r="HJ47" s="44"/>
+      <c r="HK47" s="44"/>
+      <c r="HL47" s="44"/>
+      <c r="HM47" s="44"/>
+      <c r="HN47" s="44"/>
+      <c r="HO47" s="44"/>
+      <c r="HP47" s="44"/>
+      <c r="HQ47" s="44"/>
+      <c r="HR47" s="44"/>
+      <c r="HS47" s="44"/>
+      <c r="HT47" s="44"/>
+      <c r="HU47" s="44"/>
+      <c r="HV47" s="44"/>
+      <c r="HW47" s="44"/>
+      <c r="HX47" s="44"/>
+      <c r="HY47" s="44"/>
+      <c r="HZ47" s="44"/>
+      <c r="IA47" s="44"/>
+      <c r="IB47" s="44"/>
+      <c r="IC47" s="44"/>
+      <c r="ID47" s="44"/>
+      <c r="IE47" s="44"/>
+      <c r="IF47" s="44"/>
+      <c r="IG47" s="44"/>
+      <c r="IH47" s="44"/>
+      <c r="II47" s="44"/>
+      <c r="IJ47" s="44"/>
+      <c r="IK47" s="44"/>
+      <c r="IL47" s="44"/>
+      <c r="IM47" s="44"/>
+      <c r="IN47" s="44"/>
+      <c r="IO47" s="44"/>
+      <c r="IP47" s="44"/>
+      <c r="IQ47" s="44"/>
+      <c r="IR47" s="44"/>
+      <c r="IS47" s="44"/>
+      <c r="IT47" s="44"/>
+      <c r="IU47" s="44"/>
+      <c r="IV47" s="44"/>
+      <c r="IW47" s="44"/>
+      <c r="IX47" s="44"/>
+      <c r="IY47" s="44"/>
+      <c r="IZ47" s="44"/>
+    </row>
+    <row r="48" spans="1:260" s="45" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="B48" s="9"/>
+      <c r="C48" s="10">
+        <v>8</v>
+      </c>
+      <c r="D48" s="10"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="10"/>
+      <c r="H48" s="10"/>
+      <c r="I48" s="10"/>
+      <c r="J48" s="10"/>
+      <c r="K48" s="36"/>
+      <c r="L48" s="38" t="s">
+        <v>170</v>
+      </c>
+      <c r="M48" s="44"/>
+      <c r="N48" s="44"/>
+      <c r="O48" s="44"/>
+      <c r="P48" s="44"/>
+      <c r="Q48" s="44"/>
+      <c r="R48" s="44"/>
+      <c r="S48" s="44"/>
+      <c r="T48" s="44"/>
+      <c r="U48" s="44"/>
+      <c r="V48" s="44"/>
+      <c r="W48" s="44"/>
+      <c r="X48" s="44"/>
+      <c r="Y48" s="44"/>
+      <c r="Z48" s="44"/>
+      <c r="AA48" s="44"/>
+      <c r="AB48" s="44"/>
+      <c r="AC48" s="44"/>
+      <c r="AD48" s="44"/>
+      <c r="AE48" s="44"/>
+      <c r="AF48" s="44"/>
+      <c r="AG48" s="44"/>
+      <c r="AH48" s="44"/>
+      <c r="AI48" s="44"/>
+      <c r="AJ48" s="44"/>
+      <c r="AK48" s="44"/>
+      <c r="AL48" s="44"/>
+      <c r="AM48" s="44"/>
+      <c r="AN48" s="44"/>
+      <c r="AO48" s="44"/>
+      <c r="AP48" s="44"/>
+      <c r="AQ48" s="44"/>
+      <c r="AR48" s="44"/>
+      <c r="AS48" s="44"/>
+      <c r="AT48" s="44"/>
+      <c r="AU48" s="44"/>
+      <c r="AV48" s="44"/>
+      <c r="AW48" s="44"/>
+      <c r="AX48" s="44"/>
+      <c r="AY48" s="44"/>
+      <c r="AZ48" s="44"/>
+      <c r="BA48" s="44"/>
+      <c r="BB48" s="44"/>
+      <c r="BC48" s="44"/>
+      <c r="BD48" s="44"/>
+      <c r="BE48" s="44"/>
+      <c r="BF48" s="44"/>
+      <c r="BG48" s="44"/>
+      <c r="BH48" s="44"/>
+      <c r="BI48" s="44"/>
+      <c r="BJ48" s="44"/>
+      <c r="BK48" s="44"/>
+      <c r="BL48" s="44"/>
+      <c r="BM48" s="44"/>
+      <c r="BN48" s="44"/>
+      <c r="BO48" s="44"/>
+      <c r="BP48" s="44"/>
+      <c r="BQ48" s="44"/>
+      <c r="BR48" s="44"/>
+      <c r="BS48" s="44"/>
+      <c r="BT48" s="44"/>
+      <c r="BU48" s="44"/>
+      <c r="BV48" s="44"/>
+      <c r="BW48" s="44"/>
+      <c r="BX48" s="44"/>
+      <c r="BY48" s="44"/>
+      <c r="BZ48" s="44"/>
+      <c r="CA48" s="44"/>
+      <c r="CB48" s="44"/>
+      <c r="CC48" s="44"/>
+      <c r="CD48" s="44"/>
+      <c r="CE48" s="44"/>
+      <c r="CF48" s="44"/>
+      <c r="CG48" s="44"/>
+      <c r="CH48" s="44"/>
+      <c r="CI48" s="44"/>
+      <c r="CJ48" s="44"/>
+      <c r="CK48" s="44"/>
+      <c r="CL48" s="44"/>
+      <c r="CM48" s="44"/>
+      <c r="CN48" s="44"/>
+      <c r="CO48" s="44"/>
+      <c r="CP48" s="44"/>
+      <c r="CQ48" s="44"/>
+      <c r="CR48" s="44"/>
+      <c r="CS48" s="44"/>
+      <c r="CT48" s="44"/>
+      <c r="CU48" s="44"/>
+      <c r="CV48" s="44"/>
+      <c r="CW48" s="44"/>
+      <c r="CX48" s="44"/>
+      <c r="CY48" s="44"/>
+      <c r="CZ48" s="44"/>
+      <c r="DA48" s="44"/>
+      <c r="DB48" s="44"/>
+      <c r="DC48" s="44"/>
+      <c r="DD48" s="44"/>
+      <c r="DE48" s="44"/>
+      <c r="DF48" s="44"/>
+      <c r="DG48" s="44"/>
+      <c r="DH48" s="44"/>
+      <c r="DI48" s="44"/>
+      <c r="DJ48" s="44"/>
+      <c r="DK48" s="44"/>
+      <c r="DL48" s="44"/>
+      <c r="DM48" s="44"/>
+      <c r="DN48" s="44"/>
+      <c r="DO48" s="44"/>
+      <c r="DP48" s="44"/>
+      <c r="DQ48" s="44"/>
+      <c r="DR48" s="44"/>
+      <c r="DS48" s="44"/>
+      <c r="DT48" s="44"/>
+      <c r="DU48" s="44"/>
+      <c r="DV48" s="44"/>
+      <c r="DW48" s="44"/>
+      <c r="DX48" s="44"/>
+      <c r="DY48" s="44"/>
+      <c r="DZ48" s="44"/>
+      <c r="EA48" s="44"/>
+      <c r="EB48" s="44"/>
+      <c r="EC48" s="44"/>
+      <c r="ED48" s="44"/>
+      <c r="EE48" s="44"/>
+      <c r="EF48" s="44"/>
+      <c r="EG48" s="44"/>
+      <c r="EH48" s="44"/>
+      <c r="EI48" s="44"/>
+      <c r="EJ48" s="44"/>
+      <c r="EK48" s="44"/>
+      <c r="EL48" s="44"/>
+      <c r="EM48" s="44"/>
+      <c r="EN48" s="44"/>
+      <c r="EO48" s="44"/>
+      <c r="EP48" s="44"/>
+      <c r="EQ48" s="44"/>
+      <c r="ER48" s="44"/>
+      <c r="ES48" s="44"/>
+      <c r="ET48" s="44"/>
+      <c r="EU48" s="44"/>
+      <c r="EV48" s="44"/>
+      <c r="EW48" s="44"/>
+      <c r="EX48" s="44"/>
+      <c r="EY48" s="44"/>
+      <c r="EZ48" s="44"/>
+      <c r="FA48" s="44"/>
+      <c r="FB48" s="44"/>
+      <c r="FC48" s="44"/>
+      <c r="FD48" s="44"/>
+      <c r="FE48" s="44"/>
+      <c r="FF48" s="44"/>
+      <c r="FG48" s="44"/>
+      <c r="FH48" s="44"/>
+      <c r="FI48" s="44"/>
+      <c r="FJ48" s="44"/>
+      <c r="FK48" s="44"/>
+      <c r="FL48" s="44"/>
+      <c r="FM48" s="44"/>
+      <c r="FN48" s="44"/>
+      <c r="FO48" s="44"/>
+      <c r="FP48" s="44"/>
+      <c r="FQ48" s="44"/>
+      <c r="FR48" s="44"/>
+      <c r="FS48" s="44"/>
+      <c r="FT48" s="44"/>
+      <c r="FU48" s="44"/>
+      <c r="FV48" s="44"/>
+      <c r="FW48" s="44"/>
+      <c r="FX48" s="44"/>
+      <c r="FY48" s="44"/>
+      <c r="FZ48" s="44"/>
+      <c r="GA48" s="44"/>
+      <c r="GB48" s="44"/>
+      <c r="GC48" s="44"/>
+      <c r="GD48" s="44"/>
+      <c r="GE48" s="44"/>
+      <c r="GF48" s="44"/>
+      <c r="GG48" s="44"/>
+      <c r="GH48" s="44"/>
+      <c r="GI48" s="44"/>
+      <c r="GJ48" s="44"/>
+      <c r="GK48" s="44"/>
+      <c r="GL48" s="44"/>
+      <c r="GM48" s="44"/>
+      <c r="GN48" s="44"/>
+      <c r="GO48" s="44"/>
+      <c r="GP48" s="44"/>
+      <c r="GQ48" s="44"/>
+      <c r="GR48" s="44"/>
+      <c r="GS48" s="44"/>
+      <c r="GT48" s="44"/>
+      <c r="GU48" s="44"/>
+      <c r="GV48" s="44"/>
+      <c r="GW48" s="44"/>
+      <c r="GX48" s="44"/>
+      <c r="GY48" s="44"/>
+      <c r="GZ48" s="44"/>
+      <c r="HA48" s="44"/>
+      <c r="HB48" s="44"/>
+      <c r="HC48" s="44"/>
+      <c r="HD48" s="44"/>
+      <c r="HE48" s="44"/>
+      <c r="HF48" s="44"/>
+      <c r="HG48" s="44"/>
+      <c r="HH48" s="44"/>
+      <c r="HI48" s="44"/>
+      <c r="HJ48" s="44"/>
+      <c r="HK48" s="44"/>
+      <c r="HL48" s="44"/>
+      <c r="HM48" s="44"/>
+      <c r="HN48" s="44"/>
+      <c r="HO48" s="44"/>
+      <c r="HP48" s="44"/>
+      <c r="HQ48" s="44"/>
+      <c r="HR48" s="44"/>
+      <c r="HS48" s="44"/>
+      <c r="HT48" s="44"/>
+      <c r="HU48" s="44"/>
+      <c r="HV48" s="44"/>
+      <c r="HW48" s="44"/>
+      <c r="HX48" s="44"/>
+      <c r="HY48" s="44"/>
+      <c r="HZ48" s="44"/>
+      <c r="IA48" s="44"/>
+      <c r="IB48" s="44"/>
+      <c r="IC48" s="44"/>
+      <c r="ID48" s="44"/>
+      <c r="IE48" s="44"/>
+      <c r="IF48" s="44"/>
+      <c r="IG48" s="44"/>
+      <c r="IH48" s="44"/>
+      <c r="II48" s="44"/>
+      <c r="IJ48" s="44"/>
+      <c r="IK48" s="44"/>
+      <c r="IL48" s="44"/>
+      <c r="IM48" s="44"/>
+      <c r="IN48" s="44"/>
+      <c r="IO48" s="44"/>
+      <c r="IP48" s="44"/>
+      <c r="IQ48" s="44"/>
+      <c r="IR48" s="44"/>
+      <c r="IS48" s="44"/>
+      <c r="IT48" s="44"/>
+      <c r="IU48" s="44"/>
+      <c r="IV48" s="44"/>
+      <c r="IW48" s="44"/>
+      <c r="IX48" s="44"/>
+      <c r="IY48" s="44"/>
+      <c r="IZ48" s="44"/>
+    </row>
+    <row r="49" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="39" t="s">
+        <v>152</v>
+      </c>
+      <c r="B49" s="9"/>
+      <c r="C49" s="10">
+        <v>8</v>
+      </c>
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="10"/>
+      <c r="H49" s="10"/>
+      <c r="I49" s="10"/>
+      <c r="J49" s="10"/>
+      <c r="K49" s="36"/>
+      <c r="L49" s="38"/>
+    </row>
+    <row r="50" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="39" t="s">
+        <v>153</v>
+      </c>
+      <c r="B50" s="9"/>
+      <c r="C50" s="10">
+        <v>6</v>
+      </c>
+      <c r="D50" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="E50" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="F50" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="G50" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="H50" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="I50" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="J50" s="10"/>
+      <c r="K50" s="10"/>
+      <c r="L50" s="37"/>
+    </row>
+    <row r="51" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="39" t="s">
+        <v>154</v>
+      </c>
+      <c r="B51" s="9"/>
+      <c r="C51" s="10">
+        <v>6</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="E51" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="F51" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="G51" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="H51" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="I51" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="J51" s="10"/>
+      <c r="K51" s="10"/>
+      <c r="L51" s="9"/>
+    </row>
+    <row r="52" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="39" t="s">
+        <v>155</v>
+      </c>
+      <c r="B52" s="9"/>
+      <c r="C52" s="10">
+        <v>6</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E52" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="F52" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="G52" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="H52" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="I52" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="J52" s="10"/>
+      <c r="K52" s="10"/>
+      <c r="L52" s="9"/>
+    </row>
+    <row r="53" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="39" t="s">
+        <v>156</v>
+      </c>
+      <c r="B53" s="9"/>
+      <c r="C53" s="10">
+        <v>8</v>
+      </c>
+      <c r="D53" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E53" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="F53" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="G53" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="H53" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="I53" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="J53" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="K53" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="L53" s="9"/>
+    </row>
+    <row r="54" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="40" t="s">
+        <v>157</v>
+      </c>
+      <c r="B54" s="32"/>
+      <c r="C54" s="33">
+        <v>6</v>
+      </c>
+      <c r="D54" s="33" t="s">
+        <v>142</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="F54" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="G54" s="33" t="s">
+        <v>144</v>
+      </c>
+      <c r="H54" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="I54" s="33" t="s">
+        <v>146</v>
+      </c>
+      <c r="J54" s="33" t="s">
+        <v>147</v>
+      </c>
+      <c r="K54" s="33"/>
+      <c r="L54" s="32"/>
+    </row>
+    <row r="55" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="41" t="s">
+        <v>158</v>
+      </c>
+      <c r="B55" s="42"/>
+      <c r="C55" s="42">
+        <v>6</v>
+      </c>
+      <c r="D55" s="42" t="s">
+        <v>149</v>
+      </c>
+      <c r="E55" s="42" t="s">
+        <v>150</v>
+      </c>
+      <c r="F55" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="G55" s="42" t="s">
         <v>161</v>
       </c>
-      <c r="B41" s="9"/>
-      <c r="C41" s="10">
-        <v>8</v>
-      </c>
-      <c r="D41" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="E41" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="F41" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="G41" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="H41" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="I41" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="J41" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="K41" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="L41" s="9"/>
-    </row>
-    <row r="42" spans="1:260" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="41" t="s">
+      <c r="H55" s="42" t="s">
         <v>162</v>
       </c>
-      <c r="B42" s="33"/>
-      <c r="C42" s="34">
+      <c r="I55" s="42" t="s">
+        <v>163</v>
+      </c>
+      <c r="J55" s="42"/>
+      <c r="K55" s="42"/>
+      <c r="L55" s="42"/>
+    </row>
+    <row r="56" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="35" t="s">
+        <v>159</v>
+      </c>
+      <c r="B56" s="34"/>
+      <c r="C56" s="34">
         <v>6</v>
       </c>
-      <c r="D42" s="34" t="s">
-        <v>147</v>
-      </c>
-      <c r="E42" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="F42" s="34" t="s">
-        <v>148</v>
-      </c>
-      <c r="G42" s="34" t="s">
-        <v>149</v>
-      </c>
-      <c r="H42" s="34" t="s">
-        <v>150</v>
-      </c>
-      <c r="I42" s="34" t="s">
-        <v>151</v>
-      </c>
-      <c r="J42" s="34" t="s">
-        <v>152</v>
-      </c>
-      <c r="K42" s="34"/>
-      <c r="L42" s="33"/>
-    </row>
-    <row r="43" spans="1:260" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="42" t="s">
-        <v>163</v>
-      </c>
-      <c r="B43" s="43"/>
-      <c r="C43" s="43">
-        <v>6</v>
-      </c>
-      <c r="D43" s="43" t="s">
-        <v>154</v>
-      </c>
-      <c r="E43" s="43" t="s">
-        <v>155</v>
-      </c>
-      <c r="F43" s="43" t="s">
+      <c r="D56" s="34" t="s">
+        <v>164</v>
+      </c>
+      <c r="E56" s="34" t="s">
         <v>165</v>
       </c>
-      <c r="G43" s="43" t="s">
+      <c r="F56" s="34" t="s">
         <v>166</v>
       </c>
-      <c r="H43" s="43" t="s">
+      <c r="G56" s="34" t="s">
         <v>167</v>
       </c>
-      <c r="I43" s="43" t="s">
+      <c r="H56" s="34" t="s">
         <v>168</v>
       </c>
-      <c r="J43" s="43"/>
-      <c r="K43" s="43"/>
-      <c r="L43" s="43"/>
-    </row>
-    <row r="44" spans="1:260" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="36" t="s">
-        <v>164</v>
-      </c>
-      <c r="B44" s="35"/>
-      <c r="C44" s="35">
-        <v>6</v>
-      </c>
-      <c r="D44" s="35" t="s">
+      <c r="I56" s="34" t="s">
         <v>169</v>
       </c>
-      <c r="E44" s="35" t="s">
-        <v>170</v>
-      </c>
-      <c r="F44" s="35" t="s">
-        <v>171</v>
-      </c>
-      <c r="G44" s="35" t="s">
-        <v>172</v>
-      </c>
-      <c r="H44" s="35" t="s">
-        <v>173</v>
-      </c>
-      <c r="I44" s="35" t="s">
-        <v>174</v>
-      </c>
-      <c r="J44" s="35"/>
-      <c r="K44" s="35"/>
-      <c r="L44" s="35"/>
-    </row>
-    <row r="45" spans="1:260" s="46" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="44"/>
-      <c r="B45" s="45"/>
-      <c r="C45" s="45"/>
-      <c r="D45" s="45"/>
-      <c r="E45" s="45"/>
-      <c r="F45" s="45"/>
-      <c r="G45" s="45"/>
-      <c r="H45" s="45"/>
-      <c r="I45" s="45"/>
-      <c r="J45" s="45"/>
-      <c r="K45" s="45"/>
-      <c r="L45" s="45"/>
-      <c r="M45" s="45"/>
-      <c r="N45" s="45"/>
-      <c r="O45" s="45"/>
-      <c r="P45" s="45"/>
-      <c r="Q45" s="45"/>
-      <c r="R45" s="45"/>
-      <c r="S45" s="45"/>
-      <c r="T45" s="45"/>
-      <c r="U45" s="45"/>
-      <c r="V45" s="45"/>
-      <c r="W45" s="45"/>
-      <c r="X45" s="45"/>
-      <c r="Y45" s="45"/>
-      <c r="Z45" s="45"/>
-      <c r="AA45" s="45"/>
-      <c r="AB45" s="45"/>
-      <c r="AC45" s="45"/>
-      <c r="AD45" s="45"/>
-      <c r="AE45" s="45"/>
-      <c r="AF45" s="45"/>
-      <c r="AG45" s="45"/>
-      <c r="AH45" s="45"/>
-      <c r="AI45" s="45"/>
-      <c r="AJ45" s="45"/>
-      <c r="AK45" s="45"/>
-      <c r="AL45" s="45"/>
-      <c r="AM45" s="45"/>
-      <c r="AN45" s="45"/>
-      <c r="AO45" s="45"/>
-      <c r="AP45" s="45"/>
-      <c r="AQ45" s="45"/>
-      <c r="AR45" s="45"/>
-      <c r="AS45" s="45"/>
-      <c r="AT45" s="45"/>
-      <c r="AU45" s="45"/>
-      <c r="AV45" s="45"/>
-      <c r="AW45" s="45"/>
-      <c r="AX45" s="45"/>
-      <c r="AY45" s="45"/>
-      <c r="AZ45" s="45"/>
-      <c r="BA45" s="45"/>
-      <c r="BB45" s="45"/>
-      <c r="BC45" s="45"/>
-      <c r="BD45" s="45"/>
-      <c r="BE45" s="45"/>
-      <c r="BF45" s="45"/>
-      <c r="BG45" s="45"/>
-      <c r="BH45" s="45"/>
-      <c r="BI45" s="45"/>
-      <c r="BJ45" s="45"/>
-      <c r="BK45" s="45"/>
-      <c r="BL45" s="45"/>
-      <c r="BM45" s="45"/>
-      <c r="BN45" s="45"/>
-      <c r="BO45" s="45"/>
-      <c r="BP45" s="45"/>
-      <c r="BQ45" s="45"/>
-      <c r="BR45" s="45"/>
-      <c r="BS45" s="45"/>
-      <c r="BT45" s="45"/>
-      <c r="BU45" s="45"/>
-      <c r="BV45" s="45"/>
-      <c r="BW45" s="45"/>
-      <c r="BX45" s="45"/>
-      <c r="BY45" s="45"/>
-      <c r="BZ45" s="45"/>
-      <c r="CA45" s="45"/>
-      <c r="CB45" s="45"/>
-      <c r="CC45" s="45"/>
-      <c r="CD45" s="45"/>
-      <c r="CE45" s="45"/>
-      <c r="CF45" s="45"/>
-      <c r="CG45" s="45"/>
-      <c r="CH45" s="45"/>
-      <c r="CI45" s="45"/>
-      <c r="CJ45" s="45"/>
-      <c r="CK45" s="45"/>
-      <c r="CL45" s="45"/>
-      <c r="CM45" s="45"/>
-      <c r="CN45" s="45"/>
-      <c r="CO45" s="45"/>
-      <c r="CP45" s="45"/>
-      <c r="CQ45" s="45"/>
-      <c r="CR45" s="45"/>
-      <c r="CS45" s="45"/>
-      <c r="CT45" s="45"/>
-      <c r="CU45" s="45"/>
-      <c r="CV45" s="45"/>
-      <c r="CW45" s="45"/>
-      <c r="CX45" s="45"/>
-      <c r="CY45" s="45"/>
-      <c r="CZ45" s="45"/>
-      <c r="DA45" s="45"/>
-      <c r="DB45" s="45"/>
-      <c r="DC45" s="45"/>
-      <c r="DD45" s="45"/>
-      <c r="DE45" s="45"/>
-      <c r="DF45" s="45"/>
-      <c r="DG45" s="45"/>
-      <c r="DH45" s="45"/>
-      <c r="DI45" s="45"/>
-      <c r="DJ45" s="45"/>
-      <c r="DK45" s="45"/>
-      <c r="DL45" s="45"/>
-      <c r="DM45" s="45"/>
-      <c r="DN45" s="45"/>
-      <c r="DO45" s="45"/>
-      <c r="DP45" s="45"/>
-      <c r="DQ45" s="45"/>
-      <c r="DR45" s="45"/>
-      <c r="DS45" s="45"/>
-      <c r="DT45" s="45"/>
-      <c r="DU45" s="45"/>
-      <c r="DV45" s="45"/>
-      <c r="DW45" s="45"/>
-      <c r="DX45" s="45"/>
-      <c r="DY45" s="45"/>
-      <c r="DZ45" s="45"/>
-      <c r="EA45" s="45"/>
-      <c r="EB45" s="45"/>
-      <c r="EC45" s="45"/>
-      <c r="ED45" s="45"/>
-      <c r="EE45" s="45"/>
-      <c r="EF45" s="45"/>
-      <c r="EG45" s="45"/>
-      <c r="EH45" s="45"/>
-      <c r="EI45" s="45"/>
-      <c r="EJ45" s="45"/>
-      <c r="EK45" s="45"/>
-      <c r="EL45" s="45"/>
-      <c r="EM45" s="45"/>
-      <c r="EN45" s="45"/>
-      <c r="EO45" s="45"/>
-      <c r="EP45" s="45"/>
-      <c r="EQ45" s="45"/>
-      <c r="ER45" s="45"/>
-      <c r="ES45" s="45"/>
-      <c r="ET45" s="45"/>
-      <c r="EU45" s="45"/>
-      <c r="EV45" s="45"/>
-      <c r="EW45" s="45"/>
-      <c r="EX45" s="45"/>
-      <c r="EY45" s="45"/>
-      <c r="EZ45" s="45"/>
-      <c r="FA45" s="45"/>
-      <c r="FB45" s="45"/>
-      <c r="FC45" s="45"/>
-      <c r="FD45" s="45"/>
-      <c r="FE45" s="45"/>
-      <c r="FF45" s="45"/>
-      <c r="FG45" s="45"/>
-      <c r="FH45" s="45"/>
-      <c r="FI45" s="45"/>
-      <c r="FJ45" s="45"/>
-      <c r="FK45" s="45"/>
-      <c r="FL45" s="45"/>
-      <c r="FM45" s="45"/>
-      <c r="FN45" s="45"/>
-      <c r="FO45" s="45"/>
-      <c r="FP45" s="45"/>
-      <c r="FQ45" s="45"/>
-      <c r="FR45" s="45"/>
-      <c r="FS45" s="45"/>
-      <c r="FT45" s="45"/>
-      <c r="FU45" s="45"/>
-      <c r="FV45" s="45"/>
-      <c r="FW45" s="45"/>
-      <c r="FX45" s="45"/>
-      <c r="FY45" s="45"/>
-      <c r="FZ45" s="45"/>
-      <c r="GA45" s="45"/>
-      <c r="GB45" s="45"/>
-      <c r="GC45" s="45"/>
-      <c r="GD45" s="45"/>
-      <c r="GE45" s="45"/>
-      <c r="GF45" s="45"/>
-      <c r="GG45" s="45"/>
-      <c r="GH45" s="45"/>
-      <c r="GI45" s="45"/>
-      <c r="GJ45" s="45"/>
-      <c r="GK45" s="45"/>
-      <c r="GL45" s="45"/>
-      <c r="GM45" s="45"/>
-      <c r="GN45" s="45"/>
-      <c r="GO45" s="45"/>
-      <c r="GP45" s="45"/>
-      <c r="GQ45" s="45"/>
-      <c r="GR45" s="45"/>
-      <c r="GS45" s="45"/>
-      <c r="GT45" s="45"/>
-      <c r="GU45" s="45"/>
-      <c r="GV45" s="45"/>
-      <c r="GW45" s="45"/>
-      <c r="GX45" s="45"/>
-      <c r="GY45" s="45"/>
-      <c r="GZ45" s="45"/>
-      <c r="HA45" s="45"/>
-      <c r="HB45" s="45"/>
-      <c r="HC45" s="45"/>
-      <c r="HD45" s="45"/>
-      <c r="HE45" s="45"/>
-      <c r="HF45" s="45"/>
-      <c r="HG45" s="45"/>
-      <c r="HH45" s="45"/>
-      <c r="HI45" s="45"/>
-      <c r="HJ45" s="45"/>
-      <c r="HK45" s="45"/>
-      <c r="HL45" s="45"/>
-      <c r="HM45" s="45"/>
-      <c r="HN45" s="45"/>
-      <c r="HO45" s="45"/>
-      <c r="HP45" s="45"/>
-      <c r="HQ45" s="45"/>
-      <c r="HR45" s="45"/>
-      <c r="HS45" s="45"/>
-      <c r="HT45" s="45"/>
-      <c r="HU45" s="45"/>
-      <c r="HV45" s="45"/>
-      <c r="HW45" s="45"/>
-      <c r="HX45" s="45"/>
-      <c r="HY45" s="45"/>
-      <c r="HZ45" s="45"/>
-      <c r="IA45" s="45"/>
-      <c r="IB45" s="45"/>
-      <c r="IC45" s="45"/>
-      <c r="ID45" s="45"/>
-      <c r="IE45" s="45"/>
-      <c r="IF45" s="45"/>
-      <c r="IG45" s="45"/>
-      <c r="IH45" s="45"/>
-      <c r="II45" s="45"/>
-      <c r="IJ45" s="45"/>
-      <c r="IK45" s="45"/>
-      <c r="IL45" s="45"/>
-      <c r="IM45" s="45"/>
-      <c r="IN45" s="45"/>
-      <c r="IO45" s="45"/>
-      <c r="IP45" s="45"/>
-      <c r="IQ45" s="45"/>
-      <c r="IR45" s="45"/>
-      <c r="IS45" s="45"/>
-      <c r="IT45" s="45"/>
-      <c r="IU45" s="45"/>
-      <c r="IV45" s="45"/>
-      <c r="IW45" s="45"/>
-      <c r="IX45" s="45"/>
-      <c r="IY45" s="45"/>
-      <c r="IZ45" s="45"/>
-    </row>
-    <row r="46" spans="1:260" s="46" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="44"/>
-      <c r="B46" s="45"/>
-      <c r="C46" s="45"/>
-      <c r="D46" s="45"/>
-      <c r="E46" s="45"/>
-      <c r="F46" s="45"/>
-      <c r="G46" s="45"/>
-      <c r="H46" s="45"/>
-      <c r="I46" s="45"/>
-      <c r="J46" s="45"/>
-      <c r="K46" s="45"/>
-      <c r="L46" s="45"/>
-      <c r="M46" s="45"/>
-      <c r="N46" s="45"/>
-      <c r="O46" s="45"/>
-      <c r="P46" s="45"/>
-      <c r="Q46" s="45"/>
-      <c r="R46" s="45"/>
-      <c r="S46" s="45"/>
-      <c r="T46" s="45"/>
-      <c r="U46" s="45"/>
-      <c r="V46" s="45"/>
-      <c r="W46" s="45"/>
-      <c r="X46" s="45"/>
-      <c r="Y46" s="45"/>
-      <c r="Z46" s="45"/>
-      <c r="AA46" s="45"/>
-      <c r="AB46" s="45"/>
-      <c r="AC46" s="45"/>
-      <c r="AD46" s="45"/>
-      <c r="AE46" s="45"/>
-      <c r="AF46" s="45"/>
-      <c r="AG46" s="45"/>
-      <c r="AH46" s="45"/>
-      <c r="AI46" s="45"/>
-      <c r="AJ46" s="45"/>
-      <c r="AK46" s="45"/>
-      <c r="AL46" s="45"/>
-      <c r="AM46" s="45"/>
-      <c r="AN46" s="45"/>
-      <c r="AO46" s="45"/>
-      <c r="AP46" s="45"/>
-      <c r="AQ46" s="45"/>
-      <c r="AR46" s="45"/>
-      <c r="AS46" s="45"/>
-      <c r="AT46" s="45"/>
-      <c r="AU46" s="45"/>
-      <c r="AV46" s="45"/>
-      <c r="AW46" s="45"/>
-      <c r="AX46" s="45"/>
-      <c r="AY46" s="45"/>
-      <c r="AZ46" s="45"/>
-      <c r="BA46" s="45"/>
-      <c r="BB46" s="45"/>
-      <c r="BC46" s="45"/>
-      <c r="BD46" s="45"/>
-      <c r="BE46" s="45"/>
-      <c r="BF46" s="45"/>
-      <c r="BG46" s="45"/>
-      <c r="BH46" s="45"/>
-      <c r="BI46" s="45"/>
-      <c r="BJ46" s="45"/>
-      <c r="BK46" s="45"/>
-      <c r="BL46" s="45"/>
-      <c r="BM46" s="45"/>
-      <c r="BN46" s="45"/>
-      <c r="BO46" s="45"/>
-      <c r="BP46" s="45"/>
-      <c r="BQ46" s="45"/>
-      <c r="BR46" s="45"/>
-      <c r="BS46" s="45"/>
-      <c r="BT46" s="45"/>
-      <c r="BU46" s="45"/>
-      <c r="BV46" s="45"/>
-      <c r="BW46" s="45"/>
-      <c r="BX46" s="45"/>
-      <c r="BY46" s="45"/>
-      <c r="BZ46" s="45"/>
-      <c r="CA46" s="45"/>
-      <c r="CB46" s="45"/>
-      <c r="CC46" s="45"/>
-      <c r="CD46" s="45"/>
-      <c r="CE46" s="45"/>
-      <c r="CF46" s="45"/>
-      <c r="CG46" s="45"/>
-      <c r="CH46" s="45"/>
-      <c r="CI46" s="45"/>
-      <c r="CJ46" s="45"/>
-      <c r="CK46" s="45"/>
-      <c r="CL46" s="45"/>
-      <c r="CM46" s="45"/>
-      <c r="CN46" s="45"/>
-      <c r="CO46" s="45"/>
-      <c r="CP46" s="45"/>
-      <c r="CQ46" s="45"/>
-      <c r="CR46" s="45"/>
-      <c r="CS46" s="45"/>
-      <c r="CT46" s="45"/>
-      <c r="CU46" s="45"/>
-      <c r="CV46" s="45"/>
-      <c r="CW46" s="45"/>
-      <c r="CX46" s="45"/>
-      <c r="CY46" s="45"/>
-      <c r="CZ46" s="45"/>
-      <c r="DA46" s="45"/>
-      <c r="DB46" s="45"/>
-      <c r="DC46" s="45"/>
-      <c r="DD46" s="45"/>
-      <c r="DE46" s="45"/>
-      <c r="DF46" s="45"/>
-      <c r="DG46" s="45"/>
-      <c r="DH46" s="45"/>
-      <c r="DI46" s="45"/>
-      <c r="DJ46" s="45"/>
-      <c r="DK46" s="45"/>
-      <c r="DL46" s="45"/>
-      <c r="DM46" s="45"/>
-      <c r="DN46" s="45"/>
-      <c r="DO46" s="45"/>
-      <c r="DP46" s="45"/>
-      <c r="DQ46" s="45"/>
-      <c r="DR46" s="45"/>
-      <c r="DS46" s="45"/>
-      <c r="DT46" s="45"/>
-      <c r="DU46" s="45"/>
-      <c r="DV46" s="45"/>
-      <c r="DW46" s="45"/>
-      <c r="DX46" s="45"/>
-      <c r="DY46" s="45"/>
-      <c r="DZ46" s="45"/>
-      <c r="EA46" s="45"/>
-      <c r="EB46" s="45"/>
-      <c r="EC46" s="45"/>
-      <c r="ED46" s="45"/>
-      <c r="EE46" s="45"/>
-      <c r="EF46" s="45"/>
-      <c r="EG46" s="45"/>
-      <c r="EH46" s="45"/>
-      <c r="EI46" s="45"/>
-      <c r="EJ46" s="45"/>
-      <c r="EK46" s="45"/>
-      <c r="EL46" s="45"/>
-      <c r="EM46" s="45"/>
-      <c r="EN46" s="45"/>
-      <c r="EO46" s="45"/>
-      <c r="EP46" s="45"/>
-      <c r="EQ46" s="45"/>
-      <c r="ER46" s="45"/>
-      <c r="ES46" s="45"/>
-      <c r="ET46" s="45"/>
-      <c r="EU46" s="45"/>
-      <c r="EV46" s="45"/>
-      <c r="EW46" s="45"/>
-      <c r="EX46" s="45"/>
-      <c r="EY46" s="45"/>
-      <c r="EZ46" s="45"/>
-      <c r="FA46" s="45"/>
-      <c r="FB46" s="45"/>
-      <c r="FC46" s="45"/>
-      <c r="FD46" s="45"/>
-      <c r="FE46" s="45"/>
-      <c r="FF46" s="45"/>
-      <c r="FG46" s="45"/>
-      <c r="FH46" s="45"/>
-      <c r="FI46" s="45"/>
-      <c r="FJ46" s="45"/>
-      <c r="FK46" s="45"/>
-      <c r="FL46" s="45"/>
-      <c r="FM46" s="45"/>
-      <c r="FN46" s="45"/>
-      <c r="FO46" s="45"/>
-      <c r="FP46" s="45"/>
-      <c r="FQ46" s="45"/>
-      <c r="FR46" s="45"/>
-      <c r="FS46" s="45"/>
-      <c r="FT46" s="45"/>
-      <c r="FU46" s="45"/>
-      <c r="FV46" s="45"/>
-      <c r="FW46" s="45"/>
-      <c r="FX46" s="45"/>
-      <c r="FY46" s="45"/>
-      <c r="FZ46" s="45"/>
-      <c r="GA46" s="45"/>
-      <c r="GB46" s="45"/>
-      <c r="GC46" s="45"/>
-      <c r="GD46" s="45"/>
-      <c r="GE46" s="45"/>
-      <c r="GF46" s="45"/>
-      <c r="GG46" s="45"/>
-      <c r="GH46" s="45"/>
-      <c r="GI46" s="45"/>
-      <c r="GJ46" s="45"/>
-      <c r="GK46" s="45"/>
-      <c r="GL46" s="45"/>
-      <c r="GM46" s="45"/>
-      <c r="GN46" s="45"/>
-      <c r="GO46" s="45"/>
-      <c r="GP46" s="45"/>
-      <c r="GQ46" s="45"/>
-      <c r="GR46" s="45"/>
-      <c r="GS46" s="45"/>
-      <c r="GT46" s="45"/>
-      <c r="GU46" s="45"/>
-      <c r="GV46" s="45"/>
-      <c r="GW46" s="45"/>
-      <c r="GX46" s="45"/>
-      <c r="GY46" s="45"/>
-      <c r="GZ46" s="45"/>
-      <c r="HA46" s="45"/>
-      <c r="HB46" s="45"/>
-      <c r="HC46" s="45"/>
-      <c r="HD46" s="45"/>
-      <c r="HE46" s="45"/>
-      <c r="HF46" s="45"/>
-      <c r="HG46" s="45"/>
-      <c r="HH46" s="45"/>
-      <c r="HI46" s="45"/>
-      <c r="HJ46" s="45"/>
-      <c r="HK46" s="45"/>
-      <c r="HL46" s="45"/>
-      <c r="HM46" s="45"/>
-      <c r="HN46" s="45"/>
-      <c r="HO46" s="45"/>
-      <c r="HP46" s="45"/>
-      <c r="HQ46" s="45"/>
-      <c r="HR46" s="45"/>
-      <c r="HS46" s="45"/>
-      <c r="HT46" s="45"/>
-      <c r="HU46" s="45"/>
-      <c r="HV46" s="45"/>
-      <c r="HW46" s="45"/>
-      <c r="HX46" s="45"/>
-      <c r="HY46" s="45"/>
-      <c r="HZ46" s="45"/>
-      <c r="IA46" s="45"/>
-      <c r="IB46" s="45"/>
-      <c r="IC46" s="45"/>
-      <c r="ID46" s="45"/>
-      <c r="IE46" s="45"/>
-      <c r="IF46" s="45"/>
-      <c r="IG46" s="45"/>
-      <c r="IH46" s="45"/>
-      <c r="II46" s="45"/>
-      <c r="IJ46" s="45"/>
-      <c r="IK46" s="45"/>
-      <c r="IL46" s="45"/>
-      <c r="IM46" s="45"/>
-      <c r="IN46" s="45"/>
-      <c r="IO46" s="45"/>
-      <c r="IP46" s="45"/>
-      <c r="IQ46" s="45"/>
-      <c r="IR46" s="45"/>
-      <c r="IS46" s="45"/>
-      <c r="IT46" s="45"/>
-      <c r="IU46" s="45"/>
-      <c r="IV46" s="45"/>
-      <c r="IW46" s="45"/>
-      <c r="IX46" s="45"/>
-      <c r="IY46" s="45"/>
-      <c r="IZ46" s="45"/>
+      <c r="J56" s="34"/>
+      <c r="K56" s="34"/>
+      <c r="L56" s="34"/>
+    </row>
+    <row r="57" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="43"/>
+      <c r="B57" s="44"/>
+      <c r="C57" s="44"/>
+      <c r="D57" s="44"/>
+      <c r="E57" s="44"/>
+      <c r="F57" s="44"/>
+      <c r="G57" s="44"/>
+      <c r="H57" s="44"/>
+      <c r="I57" s="44"/>
+      <c r="J57" s="44"/>
+      <c r="K57" s="44"/>
+      <c r="L57" s="44"/>
+    </row>
+    <row r="58" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="43"/>
+      <c r="B58" s="44"/>
+      <c r="C58" s="44"/>
+      <c r="D58" s="44"/>
+      <c r="E58" s="44"/>
+      <c r="F58" s="44"/>
+      <c r="G58" s="44"/>
+      <c r="H58" s="44"/>
+      <c r="I58" s="44"/>
+      <c r="J58" s="44"/>
+      <c r="K58" s="44"/>
+      <c r="L58" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5704,37 +6680,37 @@
   <sheetData>
     <row r="1" spans="1:1" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="22" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="24" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="32" t="s">
-        <v>121</v>
+      <c r="A7" s="31" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -5757,7 +6733,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.19921875" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5768,10 +6744,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" s="30"/>
+      <c r="A1" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="46"/>
     </row>
     <row r="2" spans="1:2" ht="20.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
@@ -5783,50 +6759,50 @@
     </row>
     <row r="3" spans="1:2" ht="20.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -5863,21 +6839,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
+      <c r="A1" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
     </row>
     <row r="2" spans="1:9" ht="20.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B2" s="7">
         <v>0</v>
@@ -5906,23 +6882,23 @@
     </row>
     <row r="3" spans="1:9" ht="20.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>84</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>87</v>
       </c>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
       <c r="I3" s="9" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -5939,12 +6915,26 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="12.95" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>